<commit_message>
update to BOM and purchases
</commit_message>
<xml_diff>
--- a/Minidrop build and test/Our aid documents and purchases/BOM.xlsx
+++ b/Minidrop build and test/Our aid documents and purchases/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twenzel/Documents/GitHub/OpenMicrofluidics/Minidrop build and test/Our aid documents and purchases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B858B4-F8EF-0A4C-ADED-26278D83D340}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78842B60-3E77-A040-884A-A1473A9985DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31520" yWindow="-2440" windowWidth="30700" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="1060" windowWidth="30700" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="149">
   <si>
     <r>
       <rPr>
@@ -70,7 +70,29 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>3S</t>
+      <t>Micro SD Card 8GD SD10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>SDSDQUAN-008G-G4A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Amazon</t>
     </r>
     <r>
       <rPr>
@@ -88,60 +110,18 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>OO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF484848"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Newall&lt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Element14</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Micro SD Card 8GD SD10</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>SDSDQUAN-008G-G4A</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Amazon</t>
+      <t>com</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Raspbeny P</t>
     </r>
     <r>
       <rPr>
@@ -150,35 +130,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>com</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Raspbeny P</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF8E8E8E"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>i</t>
     </r>
     <r>
@@ -200,17 +151,6 @@
         <family val="2"/>
       </rPr>
       <t>49Y1712</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Newall&lt; Element14</t>
     </r>
   </si>
   <si>
@@ -299,11 +239,111 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>18</t>
+        <color rgb="FF484848"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Hi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF727272"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF484848"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tech </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Pneumatics</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Smart producls</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">4-phase </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF727272"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">5VDC </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>unipolar stepper motor</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Jameco</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>EasyDriver stepper motor driver</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>14</t>
     </r>
     <r>
       <rPr>
@@ -321,19 +361,43 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>SO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Par1&lt;er </t>
-    </r>
+      <t>9S</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Custom PCB</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NIA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>RoyalCircuit Solutions</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -341,7 +405,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Hanna</t>
+      <t>Dig</t>
     </r>
     <r>
       <rPr>
@@ -350,16 +414,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">fin </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Precision Fluidi</t>
+      <t>iKey</t>
     </r>
   </si>
   <si>
@@ -370,7 +425,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Hi</t>
+      <t>DC</t>
     </r>
     <r>
       <rPr>
@@ -379,8 +434,52 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>-</t>
-    </r>
+      <t xml:space="preserve">/DC </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>converter</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Solenoid driver DRV104</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DigiKey</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF727272"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1S</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -388,27 +487,65 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Tech </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Pneumatics</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>6S</t>
+      <t>LD1117V50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF727272"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">-DG </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">transistor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF727272"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(tC3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>on PCB)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>68Kohm RES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>PPC68</t>
     </r>
     <r>
       <rPr>
@@ -422,218 +559,12 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>OO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>6S</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA3A3A3"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>00</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Smart producls</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">4-phase </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
         <color rgb="FF727272"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">5VDC </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>unipolar stepper motor</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Jameco</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>EasyDriver stepper motor driver</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>14</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA3A3A3"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>9S</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Spar1&lt;Fun</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Custom PCB</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NIA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2S</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA3A3A3"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>OO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>RoyalCircuit Solutions</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>6S.74</t>
-    </r>
-  </si>
-  <si>
+      <t>1KZTR</t>
+    </r>
     <r>
       <rPr>
         <sz val="12"/>
@@ -641,8 +572,10 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Dig</t>
-    </r>
+      <t>-ND</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -650,10 +583,101 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>iKey</t>
-    </r>
-  </si>
-  <si>
+      <t xml:space="preserve">1uF </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>CAP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>470pF CAP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">22ohm RES </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF727272"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(RS </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>on PCB)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2.1mm BarrelJack Connector</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Adafruit</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2N4401transistor</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">40-PIN </t>
+    </r>
     <r>
       <rPr>
         <sz val="12"/>
@@ -661,8 +685,19 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>DC</t>
-    </r>
+      <t xml:space="preserve">IDC </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>connector</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -670,78 +705,38 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">/DC </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>converter</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Solenoid driver DRV104</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>S</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA3A3A3"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>62</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>DigiKey</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF727272"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1S</t>
+      <t xml:space="preserve">1N4007 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DIODE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Disc1 magnet N42</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>K&amp;J Magnetics</t>
     </r>
   </si>
   <si>
@@ -752,411 +747,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>LD1117V50</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF727272"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">-DG </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">transistor </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF727272"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(tC3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>on PCB)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>O</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF8E8E8E"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>S7</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF8E8E8E"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>S7</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>68Kohm RES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>PPC68</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA3A3A3"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF727272"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1KZTR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF484848"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-ND</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>O</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA3A3A3"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>S2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF727272"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">1uF </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>CAP</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>470pF CAP</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">22ohm RES </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF727272"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(RS </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>on PCB)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2.1mm BarrelJack Connector</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF484848"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA3A3A3"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2S</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF8E8E8E"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>7S</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Adafruit</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2N4401transistor</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">40-PIN </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF484848"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">IDC </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>connector</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF727272"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">1N4007 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>DIODE</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Disc1 magnet N42</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>K&amp;J Magnetics</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF484848"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t xml:space="preserve">Disc2 </t>
     </r>
     <r>
@@ -1167,35 +757,6 @@
         <family val="2"/>
       </rPr>
       <t>magnet N42</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF727272"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>18</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA3A3A3"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>9S</t>
     </r>
   </si>
   <si>
@@ -1493,35 +1054,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>O</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF8E8E8E"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>OS9</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t xml:space="preserve">Nut </t>
     </r>
     <r>
@@ -1608,35 +1140,6 @@
         <family val="1"/>
       </rPr>
       <t>#4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA3A3A3"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>06S</t>
     </r>
   </si>
   <si>
@@ -2722,9 +2225,6 @@
     <t>V800-30 W/K</t>
   </si>
   <si>
-    <t>rriX7 Solenoid valve</t>
-  </si>
-  <si>
     <t>Airtrol Regulator</t>
   </si>
   <si>
@@ -3098,6 +2598,76 @@
   </si>
   <si>
     <t>Dimensions: 1/4" dia. x 3/32" thick</t>
+  </si>
+  <si>
+    <t>Newark Element14</t>
+  </si>
+  <si>
+    <t>SparkFun</t>
+  </si>
+  <si>
+    <t>mouser</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA3A3A3"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Parker Hannifin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF727272"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF606060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Precision Fluidics</t>
+    </r>
+  </si>
+  <si>
+    <t>MX7 solenoid activated poppet valve</t>
   </si>
 </sst>
 </file>
@@ -3335,7 +2905,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3396,9 +2966,6 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3450,9 +3017,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3462,9 +3026,6 @@
     <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3513,9 +3074,6 @@
     <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3525,55 +3083,82 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3600,13 +3185,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>939800</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3644,13 +3229,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3149600</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>965200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3688,13 +3273,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>965200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3086100</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3732,13 +3317,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>977900</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>939800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1981200</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3776,13 +3361,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4889500</xdr:colOff>
-      <xdr:row>125</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3820,13 +3405,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4965700</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>749300</xdr:colOff>
-      <xdr:row>126</xdr:row>
+      <xdr:row>127</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3864,13 +3449,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>126</xdr:row>
+      <xdr:row>127</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3908,13 +3493,13 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>442</xdr:row>
+      <xdr:row>443</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>449</xdr:row>
+      <xdr:row>450</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3952,13 +3537,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>288</xdr:row>
+      <xdr:row>289</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>295</xdr:row>
+      <xdr:row>296</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3996,13 +3581,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>127</xdr:row>
+      <xdr:row>128</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1270000</xdr:colOff>
-      <xdr:row>134</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4040,13 +3625,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1562100</xdr:colOff>
-      <xdr:row>127</xdr:row>
+      <xdr:row>128</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3022600</xdr:colOff>
-      <xdr:row>134</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4084,13 +3669,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3225800</xdr:colOff>
-      <xdr:row>127</xdr:row>
+      <xdr:row>128</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4699000</xdr:colOff>
-      <xdr:row>134</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4448,10 +4033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="C10" sqref="C10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.3984375" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4463,7 +4048,7 @@
     <col min="5" max="6" width="20.796875" customWidth="1"/>
     <col min="7" max="7" width="17.3984375" customWidth="1"/>
     <col min="8" max="8" width="47.796875" customWidth="1"/>
-    <col min="9" max="9" width="33.3984375" style="54" customWidth="1"/>
+    <col min="9" max="9" width="33.3984375" style="51" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -4473,64 +4058,64 @@
     </row>
     <row r="2" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="F2" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="G2" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="H2" t="s">
-        <v>128</v>
-      </c>
-      <c r="I2" s="54" t="s">
-        <v>132</v>
+        <v>108</v>
+      </c>
+      <c r="I2" s="51" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="18" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="21">
+      <c r="A3" s="20">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="23">
+      <c r="D3" s="66"/>
+      <c r="E3" s="22">
         <v>35</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="20">
         <v>1</v>
       </c>
-      <c r="G3" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="55"/>
+      <c r="G3" s="21">
+        <v>35</v>
+      </c>
+      <c r="H3" s="83" t="s">
+        <v>143</v>
+      </c>
+      <c r="I3" s="52"/>
     </row>
     <row r="4" spans="1:9" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="19">
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="72" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="72"/>
-      <c r="E4" s="20">
+        <v>3</v>
+      </c>
+      <c r="C4" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="67"/>
+      <c r="E4" s="16">
         <v>9.89</v>
       </c>
       <c r="F4" s="17">
@@ -4540,21 +4125,21 @@
         <v>9.89</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="55"/>
+        <v>5</v>
+      </c>
+      <c r="I4" s="52"/>
     </row>
     <row r="5" spans="1:9" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="19">
         <v>3</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="72"/>
+        <v>6</v>
+      </c>
+      <c r="C5" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="67"/>
       <c r="E5" s="16">
         <v>60</v>
       </c>
@@ -4564,23 +4149,25 @@
       <c r="G5" s="16">
         <v>60</v>
       </c>
-      <c r="H5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="55"/>
+      <c r="H5" s="62" t="s">
+        <v>143</v>
+      </c>
+      <c r="I5" s="52" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="65" t="s">
-        <v>122</v>
-      </c>
-      <c r="D6" s="66"/>
-      <c r="E6" s="5">
+        <v>8</v>
+      </c>
+      <c r="C6" s="68" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="69"/>
+      <c r="E6" s="7">
         <v>1.54</v>
       </c>
       <c r="F6" s="6">
@@ -4590,45 +4177,45 @@
         <v>1.54</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="72" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="72"/>
+        <v>11</v>
+      </c>
+      <c r="C7" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="67"/>
       <c r="E7" s="16">
         <v>18.5</v>
       </c>
       <c r="F7" s="17">
         <v>1</v>
       </c>
-      <c r="G7" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="55"/>
+      <c r="G7" s="14">
+        <v>18.5</v>
+      </c>
+      <c r="H7" s="84" t="s">
+        <v>143</v>
+      </c>
+      <c r="I7" s="52"/>
     </row>
     <row r="8" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="65" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" s="66"/>
+      <c r="B8" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="69"/>
       <c r="E8" s="7">
         <v>42</v>
       </c>
@@ -4639,20 +4226,20 @@
         <v>84</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>17</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" s="65" t="s">
-        <v>100</v>
-      </c>
-      <c r="D9" s="66"/>
+      <c r="B9" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="69"/>
       <c r="E9" s="7">
         <v>36.299999999999997</v>
       </c>
@@ -4663,31 +4250,31 @@
         <v>72.599999999999994</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="65" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" s="66"/>
-      <c r="E10" s="4" t="s">
-        <v>19</v>
+      <c r="B10" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="69"/>
+      <c r="E10" s="61">
+        <v>65</v>
       </c>
       <c r="F10" s="9">
         <v>1</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>20</v>
+      <c r="G10" s="4">
+        <v>65</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -4695,13 +4282,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="78">
+        <v>15</v>
+      </c>
+      <c r="C11" s="70">
         <v>237825</v>
       </c>
-      <c r="D11" s="78"/>
-      <c r="E11" s="5">
+      <c r="D11" s="70"/>
+      <c r="E11" s="7">
         <v>9.9499999999999993</v>
       </c>
       <c r="F11" s="6">
@@ -4710,96 +4297,98 @@
       <c r="G11" s="7">
         <v>9.9499999999999993</v>
       </c>
-      <c r="H11" s="24" t="s">
-        <v>120</v>
+      <c r="H11" s="23" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="31">
+      <c r="A12" s="30">
         <v>10</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C12" s="71" t="s">
-        <v>119</v>
-      </c>
-      <c r="D12" s="72"/>
-      <c r="E12" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="32">
+        <v>99</v>
+      </c>
+      <c r="D12" s="67"/>
+      <c r="E12" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="31">
         <v>1</v>
       </c>
-      <c r="G12" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="55"/>
+      <c r="G12" s="15">
+        <v>14.95</v>
+      </c>
+      <c r="H12" s="62" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" s="52" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="13" spans="1:9" s="18" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="31">
+      <c r="A13" s="30">
         <v>11</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="72" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="72"/>
+        <v>19</v>
+      </c>
+      <c r="C13" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="67"/>
       <c r="E13" s="16">
         <v>25</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="31">
         <v>1</v>
       </c>
-      <c r="G13" s="14" t="s">
-        <v>29</v>
+      <c r="G13" s="14">
+        <v>25</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="55"/>
-    </row>
-    <row r="14" spans="1:9" s="30" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="25">
+        <v>21</v>
+      </c>
+      <c r="I13" s="52"/>
+    </row>
+    <row r="14" spans="1:9" s="29" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="24">
         <v>12</v>
       </c>
-      <c r="B14" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" s="74" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" s="75"/>
-      <c r="E14" s="28">
+      <c r="B14" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="72" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="73"/>
+      <c r="E14" s="27">
         <v>32.869999999999997</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="28">
         <v>2</v>
       </c>
-      <c r="G14" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" s="56"/>
+      <c r="G14" s="25">
+        <v>65.739999999999995</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="53"/>
     </row>
     <row r="15" spans="1:9" s="18" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="31">
+      <c r="A15" s="30">
         <v>13</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C15" s="71" t="s">
-        <v>116</v>
-      </c>
-      <c r="D15" s="72"/>
+        <v>96</v>
+      </c>
+      <c r="D15" s="67"/>
       <c r="E15" s="16">
         <v>10.68</v>
       </c>
@@ -4810,23 +4399,25 @@
         <v>21.36</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="55"/>
+        <v>22</v>
+      </c>
+      <c r="I15" s="52" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="16" spans="1:9" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="31">
+      <c r="A16" s="30">
         <v>14</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C16" s="71" t="s">
-        <v>107</v>
-      </c>
-      <c r="D16" s="72"/>
-      <c r="E16" s="14" t="s">
-        <v>35</v>
+        <v>87</v>
+      </c>
+      <c r="D16" s="67"/>
+      <c r="E16" s="63">
+        <v>5.62</v>
       </c>
       <c r="F16" s="17">
         <v>2</v>
@@ -4835,48 +4426,50 @@
         <v>11.24</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="I16" s="55"/>
-    </row>
-    <row r="17" spans="1:10" s="37" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="76" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" s="77"/>
-      <c r="E17" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="36">
+        <v>25</v>
+      </c>
+      <c r="I16" s="52" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="36" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="74" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="75"/>
+      <c r="E17" s="64">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F17" s="35">
         <v>1</v>
       </c>
-      <c r="G17" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" s="57"/>
+      <c r="G17" s="34">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="54"/>
     </row>
     <row r="18" spans="1:10" s="18" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="31">
+      <c r="A18" s="30">
         <v>16</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="72" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="72"/>
-      <c r="E18" s="15" t="s">
-        <v>43</v>
+        <v>28</v>
+      </c>
+      <c r="C18" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="67"/>
+      <c r="E18" s="63" t="s">
+        <v>146</v>
       </c>
       <c r="F18" s="17">
         <v>4</v>
@@ -4885,21 +4478,23 @@
         <v>2.08</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="I18" s="55"/>
+        <v>25</v>
+      </c>
+      <c r="I18" s="52" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="19" spans="1:10" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="31">
+      <c r="A19" s="30">
         <v>17</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C19" s="71" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" s="72"/>
+        <v>88</v>
+      </c>
+      <c r="D19" s="67"/>
       <c r="E19" s="16">
         <v>0.11</v>
       </c>
@@ -4910,172 +4505,182 @@
         <v>0.22</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="I19" s="55"/>
-    </row>
-    <row r="20" spans="1:10" s="30" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="25">
+        <v>25</v>
+      </c>
+      <c r="I19" s="52" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="29" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="24">
         <v>18</v>
       </c>
-      <c r="B20" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="74" t="s">
-        <v>109</v>
-      </c>
-      <c r="D20" s="75"/>
-      <c r="E20" s="38">
+      <c r="B20" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="72" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="73"/>
+      <c r="E20" s="27">
         <v>0.25</v>
       </c>
-      <c r="F20" s="29">
+      <c r="F20" s="28">
         <v>2</v>
       </c>
-      <c r="G20" s="28">
+      <c r="G20" s="27">
         <v>0.5</v>
       </c>
-      <c r="H20" s="27" t="s">
+      <c r="H20" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="53"/>
+    </row>
+    <row r="21" spans="1:10" s="29" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="24">
+        <v>19</v>
+      </c>
+      <c r="B21" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="56"/>
-    </row>
-    <row r="21" spans="1:10" s="30" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="25">
-        <v>19</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="74" t="s">
-        <v>110</v>
-      </c>
-      <c r="D21" s="75"/>
-      <c r="E21" s="38">
+      <c r="C21" s="72" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="73"/>
+      <c r="E21" s="27">
         <v>0.1</v>
       </c>
-      <c r="F21" s="40">
+      <c r="F21" s="38">
         <v>1</v>
       </c>
-      <c r="G21" s="28">
+      <c r="G21" s="27">
         <v>0.1</v>
       </c>
-      <c r="H21" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="I21" s="56"/>
+      <c r="H21" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="53"/>
     </row>
     <row r="22" spans="1:10" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="19">
         <v>20</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C22" s="71" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" s="72"/>
-      <c r="E22" s="20">
+        <v>91</v>
+      </c>
+      <c r="D22" s="67"/>
+      <c r="E22" s="16">
         <v>1.25</v>
       </c>
       <c r="F22" s="17">
         <v>1</v>
       </c>
-      <c r="G22" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I22" s="55"/>
+      <c r="G22" s="15">
+        <v>1.25</v>
+      </c>
+      <c r="H22" s="62" t="s">
+        <v>144</v>
+      </c>
+      <c r="I22" s="52" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="23" spans="1:10" s="18" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="19">
         <v>21</v>
       </c>
-      <c r="B23" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="C23" s="73">
+      <c r="B23" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="76">
         <v>856</v>
       </c>
-      <c r="D23" s="73"/>
-      <c r="E23" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" s="32">
+      <c r="D23" s="76"/>
+      <c r="E23" s="63">
+        <v>3.75</v>
+      </c>
+      <c r="F23" s="31">
         <v>1</v>
       </c>
-      <c r="G23" s="15" t="s">
-        <v>49</v>
+      <c r="G23" s="15">
+        <v>3.75</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I23" s="55"/>
+        <v>34</v>
+      </c>
+      <c r="I23" s="52" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="24" spans="1:10" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="19">
         <v>22</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C24" s="71" t="s">
-        <v>112</v>
-      </c>
-      <c r="D24" s="72"/>
-      <c r="E24" s="20">
+        <v>92</v>
+      </c>
+      <c r="D24" s="67"/>
+      <c r="E24" s="16">
         <v>0.15</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="31">
         <v>1</v>
       </c>
       <c r="G24" s="16">
         <v>0.15</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="I24" s="55"/>
+        <v>25</v>
+      </c>
+      <c r="I24" s="52" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="25" spans="1:10" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="19">
         <v>23</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="73">
+        <v>36</v>
+      </c>
+      <c r="C25" s="76">
         <v>2222</v>
       </c>
-      <c r="D25" s="73"/>
-      <c r="E25" s="20">
+      <c r="D25" s="76"/>
+      <c r="E25" s="16">
         <v>1</v>
       </c>
-      <c r="F25" s="32">
+      <c r="F25" s="31">
         <v>1</v>
       </c>
-      <c r="G25" s="41">
+      <c r="G25" s="39">
         <v>1</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I25" s="55"/>
+        <v>34</v>
+      </c>
+      <c r="I25" s="52" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="26" spans="1:10" s="18" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="19">
         <v>24</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C26" s="71" t="s">
-        <v>113</v>
-      </c>
-      <c r="D26" s="72"/>
-      <c r="E26" s="20">
+        <v>93</v>
+      </c>
+      <c r="D26" s="67"/>
+      <c r="E26" s="16">
         <v>0.09</v>
       </c>
       <c r="F26" s="17">
@@ -5085,22 +4690,24 @@
         <v>0.18</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="I26" s="55"/>
+        <v>25</v>
+      </c>
+      <c r="I26" s="52" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="27" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="65" t="s">
-        <v>156</v>
-      </c>
-      <c r="D27" s="66"/>
-      <c r="E27" s="5">
+        <v>38</v>
+      </c>
+      <c r="C27" s="68" t="s">
+        <v>136</v>
+      </c>
+      <c r="D27" s="69"/>
+      <c r="E27" s="7">
         <v>0.28999999999999998</v>
       </c>
       <c r="F27" s="6">
@@ -5110,13 +4717,13 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I27" s="61" t="s">
-        <v>161</v>
-      </c>
-      <c r="J27" s="53" t="s">
-        <v>162</v>
+        <v>39</v>
+      </c>
+      <c r="I27" s="57" t="s">
+        <v>141</v>
+      </c>
+      <c r="J27" s="50" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -5124,13 +4731,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="65" t="s">
-        <v>155</v>
-      </c>
-      <c r="D28" s="66"/>
-      <c r="E28" s="5">
+        <v>40</v>
+      </c>
+      <c r="C28" s="68" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" s="69"/>
+      <c r="E28" s="7">
         <v>0.79</v>
       </c>
       <c r="F28" s="9">
@@ -5140,28 +4747,28 @@
         <v>0.79</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="I28" s="61" t="s">
-        <v>159</v>
-      </c>
-      <c r="J28" s="53" t="s">
-        <v>160</v>
+        <v>39</v>
+      </c>
+      <c r="I28" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="J28" s="50" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>27</v>
       </c>
-      <c r="B29" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="C29" s="65">
+      <c r="B29" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="68">
         <v>1952370</v>
       </c>
-      <c r="D29" s="66"/>
-      <c r="E29" s="4" t="s">
-        <v>57</v>
+      <c r="D29" s="69"/>
+      <c r="E29" s="61">
+        <v>18.95</v>
       </c>
       <c r="F29" s="9">
         <v>1</v>
@@ -5170,46 +4777,46 @@
         <v>18.95</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="49" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="46" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="42">
         <v>28</v>
       </c>
-      <c r="B30" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="64" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" s="64"/>
-      <c r="E30" s="59">
+      <c r="B30" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="77" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="77"/>
+      <c r="E30" s="49">
         <v>0.43</v>
       </c>
-      <c r="F30" s="52">
+      <c r="F30" s="49">
         <v>21.13</v>
       </c>
-      <c r="G30" s="52">
+      <c r="G30" s="49">
         <v>9.1199999999999992</v>
       </c>
-      <c r="H30" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="I30" s="58"/>
+      <c r="H30" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="I30" s="55"/>
     </row>
     <row r="31" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <v>29</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="65" t="s">
-        <v>154</v>
-      </c>
-      <c r="D31" s="66"/>
-      <c r="E31" s="5">
+        <v>44</v>
+      </c>
+      <c r="C31" s="68" t="s">
+        <v>134</v>
+      </c>
+      <c r="D31" s="69"/>
+      <c r="E31" s="7">
         <v>1.28</v>
       </c>
       <c r="F31" s="9">
@@ -5218,673 +4825,687 @@
       <c r="G31" s="8">
         <v>1.28</v>
       </c>
-      <c r="H31" s="44" t="s">
-        <v>153</v>
-      </c>
-      <c r="I31" s="61" t="s">
-        <v>157</v>
-      </c>
-      <c r="J31" s="53" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="C32" s="71" t="s">
-        <v>115</v>
-      </c>
-      <c r="D32" s="72"/>
-      <c r="E32" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="F32" s="17">
+      <c r="H31" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="I31" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="J31" s="50" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="65"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="57"/>
+      <c r="J32" s="50"/>
+    </row>
+    <row r="33" spans="1:9" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="67"/>
+      <c r="E33" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" s="17">
         <v>1</v>
       </c>
-      <c r="G32" s="41">
+      <c r="G33" s="39">
         <v>1.25</v>
       </c>
-      <c r="H32" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I32" s="55"/>
-    </row>
-    <row r="33" spans="1:9" s="49" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="45">
+      <c r="H33" s="62" t="s">
+        <v>144</v>
+      </c>
+      <c r="I33" s="52" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="46" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="42">
         <v>30</v>
       </c>
-      <c r="B33" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="69">
+      <c r="B34" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="78">
         <v>2094346</v>
       </c>
-      <c r="D33" s="69"/>
-      <c r="E33" s="47">
+      <c r="D34" s="78"/>
+      <c r="E34" s="44">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="F33" s="48">
+      <c r="F34" s="45">
         <v>8</v>
       </c>
-      <c r="G33" s="47">
+      <c r="G34" s="44">
         <v>0.55200000000000005</v>
       </c>
-      <c r="H33" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="I33" s="58"/>
-    </row>
-    <row r="34" spans="1:9" s="49" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="45">
+      <c r="H34" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="I34" s="55"/>
+    </row>
+    <row r="35" spans="1:9" s="46" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="42">
         <v>31</v>
       </c>
-      <c r="B34" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" s="69">
+      <c r="B35" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="78">
         <v>106797</v>
       </c>
-      <c r="D34" s="69"/>
-      <c r="E34" s="47">
+      <c r="D35" s="78"/>
+      <c r="E35" s="44">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="F34" s="48">
+      <c r="F35" s="45">
         <v>4</v>
       </c>
-      <c r="G34" s="47">
+      <c r="G35" s="44">
         <v>0.316</v>
       </c>
-      <c r="H34" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="I34" s="58"/>
-    </row>
-    <row r="35" spans="1:9" s="49" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="45">
+      <c r="H35" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="55"/>
+    </row>
+    <row r="36" spans="1:9" s="46" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="42">
         <v>32</v>
       </c>
-      <c r="B35" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" s="70">
+      <c r="B36" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="79">
         <v>106810</v>
       </c>
-      <c r="D35" s="70"/>
-      <c r="E35" s="47">
+      <c r="D36" s="79"/>
+      <c r="E36" s="44">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="F35" s="48">
+      <c r="F36" s="45">
         <v>8</v>
       </c>
-      <c r="G35" s="47">
+      <c r="G36" s="44">
         <v>0.63200000000000001</v>
       </c>
-      <c r="H35" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="I35" s="58"/>
-    </row>
-    <row r="36" spans="1:9" s="49" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="45">
+      <c r="H36" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="I36" s="55"/>
+    </row>
+    <row r="37" spans="1:9" s="46" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="42">
         <v>33</v>
       </c>
-      <c r="B36" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36" s="69">
+      <c r="B37" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="78">
         <v>38173</v>
       </c>
-      <c r="D36" s="69"/>
-      <c r="E36" s="47">
+      <c r="D37" s="78"/>
+      <c r="E37" s="44">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="F36" s="48">
+      <c r="F37" s="45">
         <v>4</v>
       </c>
-      <c r="G36" s="47">
+      <c r="G37" s="44">
         <v>0.39600000000000002</v>
       </c>
-      <c r="H36" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="I36" s="58"/>
-    </row>
-    <row r="37" spans="1:9" s="49" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="45">
+      <c r="H37" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="55"/>
+    </row>
+    <row r="38" spans="1:9" s="46" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="42">
         <v>34</v>
       </c>
-      <c r="B37" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="C37" s="64">
+      <c r="B38" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="77">
         <v>51553</v>
       </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="47">
+      <c r="D38" s="77"/>
+      <c r="E38" s="44">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="F37" s="48">
+      <c r="F38" s="45">
         <v>4</v>
       </c>
-      <c r="G37" s="47">
+      <c r="G38" s="44">
         <v>0.23599999999999999</v>
       </c>
-      <c r="H37" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="I37" s="58"/>
-    </row>
-    <row r="38" spans="1:9" s="49" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="45">
+      <c r="H38" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="55"/>
+    </row>
+    <row r="39" spans="1:9" s="46" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="42">
         <v>35</v>
       </c>
-      <c r="B38" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="69">
+      <c r="B39" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="78">
         <v>40943</v>
       </c>
-      <c r="D38" s="69"/>
-      <c r="E38" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="F38" s="48">
+      <c r="D39" s="78"/>
+      <c r="E39" s="59">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F39" s="45">
         <v>4</v>
       </c>
-      <c r="G38" s="47">
+      <c r="G39" s="44">
         <v>0.23599999999999999</v>
       </c>
-      <c r="H38" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="I38" s="58"/>
-    </row>
-    <row r="39" spans="1:9" s="49" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="45">
+      <c r="H39" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="55"/>
+    </row>
+    <row r="40" spans="1:9" s="46" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="42">
         <v>36</v>
       </c>
-      <c r="B39" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="C39" s="64">
+      <c r="B40" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="77">
         <v>38165</v>
       </c>
-      <c r="D39" s="64"/>
-      <c r="E39" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="F39" s="48">
+      <c r="D40" s="77"/>
+      <c r="E40" s="59">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F40" s="45">
         <v>4</v>
       </c>
-      <c r="G39" s="47">
+      <c r="G40" s="44">
         <v>0.23599999999999999</v>
       </c>
-      <c r="H39" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="I39" s="58"/>
-    </row>
-    <row r="40" spans="1:9" s="49" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="45">
+      <c r="H40" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="55"/>
+    </row>
+    <row r="41" spans="1:9" s="46" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="42">
         <v>37</v>
       </c>
-      <c r="B40" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="C40" s="70">
+      <c r="B41" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="79">
         <v>106850</v>
       </c>
-      <c r="D40" s="70"/>
-      <c r="E40" s="47">
+      <c r="D41" s="79"/>
+      <c r="E41" s="44">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="F40" s="48">
+      <c r="F41" s="45">
         <v>2</v>
       </c>
-      <c r="G40" s="47">
+      <c r="G41" s="44">
         <v>0.11799999999999999</v>
       </c>
-      <c r="H40" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="I40" s="58"/>
-    </row>
-    <row r="41" spans="1:9" s="49" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="51">
+      <c r="H41" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="I41" s="55"/>
+    </row>
+    <row r="42" spans="1:9" s="46" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="48">
         <v>38</v>
       </c>
-      <c r="B41" s="50" t="s">
-        <v>74</v>
-      </c>
-      <c r="C41" s="69">
+      <c r="B42" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="78">
         <v>106826</v>
       </c>
-      <c r="D41" s="69"/>
-      <c r="E41" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="F41" s="48">
+      <c r="D42" s="78"/>
+      <c r="E42" s="59">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="F42" s="45">
         <v>2</v>
       </c>
-      <c r="G41" s="52">
+      <c r="G42" s="49">
         <v>0.13</v>
       </c>
-      <c r="H41" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="I41" s="58"/>
-    </row>
-    <row r="42" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="3">
-        <v>39</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="65" t="s">
-        <v>137</v>
-      </c>
-      <c r="D42" s="66"/>
-      <c r="E42" s="5">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F42" s="6">
-        <v>4</v>
-      </c>
-      <c r="G42" s="12">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I42" s="54" t="s">
-        <v>140</v>
-      </c>
+      <c r="H42" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="55"/>
     </row>
     <row r="43" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="3">
+        <v>39</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="68" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" s="69"/>
+      <c r="E43" s="7">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F43" s="6">
+        <v>4</v>
+      </c>
+      <c r="G43" s="12">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I43" s="51" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="3">
         <v>40</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C43" s="65" t="s">
-        <v>134</v>
-      </c>
-      <c r="D43" s="66"/>
-      <c r="E43" s="5">
+      <c r="B44" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="68" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" s="69"/>
+      <c r="E44" s="7">
         <v>0.61</v>
       </c>
-      <c r="F43" s="6">
+      <c r="F44" s="6">
         <v>8</v>
       </c>
-      <c r="G43" s="7">
+      <c r="G44" s="7">
         <v>4.88</v>
       </c>
-      <c r="H43" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I43" s="54" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="3">
+      <c r="H44" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I44" s="51" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="3">
         <v>41</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C44" s="65" t="s">
-        <v>136</v>
-      </c>
-      <c r="D44" s="66"/>
-      <c r="E44" s="5">
+      <c r="B45" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="68" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" s="69"/>
+      <c r="E45" s="7">
         <v>0.54</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F45" s="6">
         <v>4</v>
       </c>
-      <c r="G44" s="12">
+      <c r="G45" s="12">
         <v>2.16</v>
       </c>
-      <c r="H44" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I44" s="54" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="3">
+      <c r="H45" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I45" s="51" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="3">
         <v>42</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C45" s="65" t="s">
-        <v>135</v>
-      </c>
-      <c r="D45" s="66"/>
-      <c r="E45" s="5">
+      <c r="B46" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" s="68" t="s">
+        <v>115</v>
+      </c>
+      <c r="D46" s="69"/>
+      <c r="E46" s="7">
         <v>0.27</v>
-      </c>
-      <c r="F45" s="6">
-        <v>2</v>
-      </c>
-      <c r="G45" s="7">
-        <v>0.54</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I45" s="54" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="3">
-        <v>43</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C46" s="66" t="s">
-        <v>144</v>
-      </c>
-      <c r="D46" s="66"/>
-      <c r="E46" s="11">
-        <v>0.41799999999999998</v>
       </c>
       <c r="F46" s="6">
         <v>2</v>
       </c>
-      <c r="G46" s="11">
-        <v>0.83599999999999997</v>
+      <c r="G46" s="7">
+        <v>0.54</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="I46" s="54" t="s">
-        <v>145</v>
+        <v>58</v>
+      </c>
+      <c r="I46" s="51" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3">
+        <v>43</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="69" t="s">
+        <v>124</v>
+      </c>
+      <c r="D47" s="69"/>
+      <c r="E47" s="11">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="F47" s="6">
+        <v>2</v>
+      </c>
+      <c r="G47" s="11">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="I47" s="51" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="3">
         <v>44</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C47" s="68" t="s">
-        <v>146</v>
-      </c>
-      <c r="D47" s="66"/>
-      <c r="E47" s="11">
-        <v>0.246</v>
-      </c>
-      <c r="F47" s="6">
-        <v>4</v>
-      </c>
-      <c r="G47" s="11">
-        <v>0.98399999999999999</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="I47" s="54" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="3">
-        <v>45</v>
-      </c>
       <c r="B48" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C48" s="65" t="s">
-        <v>148</v>
-      </c>
-      <c r="D48" s="66"/>
+        <v>63</v>
+      </c>
+      <c r="C48" s="80" t="s">
+        <v>126</v>
+      </c>
+      <c r="D48" s="69"/>
       <c r="E48" s="11">
         <v>0.246</v>
       </c>
       <c r="F48" s="6">
+        <v>4</v>
+      </c>
+      <c r="G48" s="11">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I48" s="51" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="3">
+        <v>45</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="68" t="s">
+        <v>128</v>
+      </c>
+      <c r="D49" s="69"/>
+      <c r="E49" s="11">
+        <v>0.246</v>
+      </c>
+      <c r="F49" s="6">
         <v>21</v>
       </c>
-      <c r="G48" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="I48" s="54" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" s="49" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="45">
+      <c r="G49" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I49" s="51" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="46" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="42">
         <v>46</v>
       </c>
-      <c r="B49" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="C49" s="67">
+      <c r="B50" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" s="82">
         <v>2135064</v>
       </c>
-      <c r="D49" s="64"/>
-      <c r="E49" s="59">
+      <c r="D50" s="77"/>
+      <c r="E50" s="49">
         <v>2.4900000000000002</v>
       </c>
-      <c r="F49" s="48">
+      <c r="F50" s="45">
         <v>2</v>
       </c>
-      <c r="G49" s="52">
+      <c r="G50" s="49">
         <v>4.9800000000000004</v>
       </c>
-      <c r="H49" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="I49" s="58" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="3">
+      <c r="H50" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="I50" s="55" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="3">
         <v>47</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C50" s="68" t="s">
-        <v>121</v>
-      </c>
-      <c r="D50" s="66"/>
-      <c r="E50" s="6">
+      <c r="B51" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F50" s="5">
+      <c r="C51" s="80" t="s">
+        <v>101</v>
+      </c>
+      <c r="D51" s="69"/>
+      <c r="E51" s="65">
+        <v>67</v>
+      </c>
+      <c r="F51" s="5">
         <v>0.06</v>
       </c>
-      <c r="G50" s="7">
+      <c r="G51" s="7">
         <v>4.0199999999999996</v>
       </c>
-      <c r="H50" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" s="49" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="60">
+      <c r="H51" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="46" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="56">
         <v>48</v>
       </c>
-      <c r="B51" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C51" s="67" t="s">
-        <v>123</v>
-      </c>
-      <c r="D51" s="64"/>
-      <c r="E51" s="59">
+      <c r="B52" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" s="82" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="77"/>
+      <c r="E52" s="49">
         <v>9.99</v>
       </c>
-      <c r="F51" s="48">
+      <c r="F52" s="45">
         <v>1</v>
       </c>
-      <c r="G51" s="52">
+      <c r="G52" s="49">
         <v>9.99</v>
       </c>
-      <c r="H51" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="I51" s="58"/>
-    </row>
-    <row r="52" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="3">
+      <c r="H52" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="I52" s="55"/>
+    </row>
+    <row r="53" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="3">
         <v>49</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C52" s="65" t="s">
-        <v>151</v>
-      </c>
-      <c r="D52" s="66"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="6">
+      <c r="B53" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" s="69"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="6">
         <v>5</v>
       </c>
-      <c r="G52" s="10"/>
-      <c r="H52" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="I52" s="54" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" s="49" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="45">
+      <c r="G53" s="10"/>
+      <c r="H53" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I53" s="51" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="46" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="42">
         <v>50</v>
       </c>
-      <c r="B53" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="C53" s="63" t="s">
-        <v>124</v>
-      </c>
-      <c r="D53" s="64"/>
-      <c r="E53" s="50"/>
-      <c r="F53" s="62" t="s">
-        <v>13</v>
-      </c>
-      <c r="G53" s="50"/>
-      <c r="H53" s="46" t="s">
+      <c r="B54" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" s="81" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" s="77"/>
+      <c r="E54" s="47"/>
+      <c r="F54" s="58">
+        <v>5</v>
+      </c>
+      <c r="G54" s="47"/>
+      <c r="H54" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="I54" s="55"/>
+    </row>
+    <row r="55" spans="1:9" s="46" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="42">
+        <v>51</v>
+      </c>
+      <c r="B55" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" s="77" t="s">
+        <v>73</v>
+      </c>
+      <c r="D55" s="77"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
+      <c r="G55" s="47"/>
+      <c r="H55" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="I55" s="55"/>
+    </row>
+    <row r="56" spans="1:9" s="46" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="I53" s="58"/>
-    </row>
-    <row r="54" spans="1:9" s="49" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="45">
-        <v>51</v>
-      </c>
-      <c r="B54" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="C54" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="D54" s="64"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="50"/>
-      <c r="G54" s="50"/>
-      <c r="H54" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="I54" s="58"/>
-    </row>
-    <row r="55" spans="1:9" s="49" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="B55" s="46" t="s">
-        <v>95</v>
-      </c>
-      <c r="C55" s="64" t="s">
-        <v>96</v>
-      </c>
-      <c r="D55" s="64"/>
-      <c r="E55" s="50"/>
-      <c r="F55" s="50"/>
-      <c r="G55" s="50"/>
-      <c r="H55" s="46" t="s">
-        <v>97</v>
-      </c>
-      <c r="I55" s="58"/>
-    </row>
-    <row r="56" spans="1:9" ht="83" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" t="s">
-        <v>98</v>
+      <c r="D56" s="77"/>
+      <c r="E56" s="47"/>
+      <c r="F56" s="47"/>
+      <c r="G56" s="47"/>
+      <c r="H56" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="I56" s="55"/>
+    </row>
+    <row r="57" spans="1:9" ht="83" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I31" r:id="rId1" xr:uid="{A02AF87C-9527-A047-9DFE-4A7472C1BB6D}"/>

</xml_diff>

<commit_message>
extension and new projects
</commit_message>
<xml_diff>
--- a/Minidrop build and test/Our aid documents and purchases/BOM.xlsx
+++ b/Minidrop build and test/Our aid documents and purchases/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twenzel/Documents/GitHub/OpenMicrofluidics/Minidrop build and test/Our aid documents and purchases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78842B60-3E77-A040-884A-A1473A9985DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA2DD7E-6723-E148-AF50-174AA68FD0F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="1060" windowWidth="30700" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13060" yWindow="2920" windowWidth="20120" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="152">
   <si>
     <r>
       <rPr>
@@ -715,17 +715,6 @@
         <family val="2"/>
       </rPr>
       <t>DIODE</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Disc1 magnet N42</t>
     </r>
   </si>
   <si>
@@ -828,64 +817,6 @@
         <family val="2"/>
       </rPr>
       <t>Cylinder magnet</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>29</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA3A3A3"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>S</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA3A3A3"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF606060"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2S</t>
     </r>
   </si>
   <si>
@@ -2237,9 +2168,6 @@
     <t>Honeywell TruStabilily pressure sensor</t>
   </si>
   <si>
-    <t>SSCDLNN01SPGAA5</t>
-  </si>
-  <si>
     <t>296-15746-1-ND</t>
   </si>
   <si>
@@ -2249,9 +2177,6 @@
     <t>1286PH-ND</t>
   </si>
   <si>
-    <t>CF14JT22ROCT-ND</t>
-  </si>
-  <si>
     <t>PRT-00119</t>
   </si>
   <si>
@@ -2424,9 +2349,6 @@
     <t>Info</t>
   </si>
   <si>
-    <t>micro USB</t>
-  </si>
-  <si>
     <t>93505A454</t>
   </si>
   <si>
@@ -2567,9 +2489,6 @@
     <t>NE-236-304-1-45</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>K&amp;J Magnetics</t>
   </si>
   <si>
@@ -2668,6 +2587,36 @@
   </si>
   <si>
     <t>MX7 solenoid activated poppet valve</t>
+  </si>
+  <si>
+    <t>from USA</t>
+  </si>
+  <si>
+    <t>SSCDLNN015PGAA5</t>
+  </si>
+  <si>
+    <t>CF14JT22R0CT-ND</t>
+  </si>
+  <si>
+    <t>Disc1 magnet N42</t>
+  </si>
+  <si>
+    <t>from USA (coastpneumatics)</t>
+  </si>
+  <si>
+    <t>McMaster-Carr</t>
+  </si>
+  <si>
+    <t>? Difficult custom ordering process</t>
+  </si>
+  <si>
+    <t>only orders &gt;+100 pieces</t>
+  </si>
+  <si>
+    <t>we will have to use oher tubing with other connectors</t>
+  </si>
+  <si>
+    <t>already in stock</t>
   </si>
 </sst>
 </file>
@@ -2851,7 +2800,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2882,6 +2831,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -2905,7 +2860,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2942,9 +2897,6 @@
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2984,9 +2936,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3005,9 +2954,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3026,19 +2972,10 @@
     <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3050,9 +2987,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3083,6 +3017,96 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3098,67 +3122,40 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3233,8 +3230,8 @@
       <xdr:rowOff>965200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
@@ -3277,8 +3274,8 @@
       <xdr:rowOff>965200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3086100</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
@@ -3365,8 +3362,8 @@
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>4889500</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
       <xdr:row>126</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
@@ -3410,7 +3407,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
+      <xdr:colOff>1117600</xdr:colOff>
       <xdr:row>127</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
@@ -3629,8 +3626,8 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3022600</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>135</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -3673,8 +3670,8 @@
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>4699000</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>135</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -4033,22 +4030,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:D10"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.3984375" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="84" customWidth="1"/>
+    <col min="2" max="2" width="47.59765625" customWidth="1"/>
     <col min="3" max="3" width="20.796875" customWidth="1"/>
     <col min="4" max="4" width="23.3984375" customWidth="1"/>
     <col min="5" max="6" width="20.796875" customWidth="1"/>
     <col min="7" max="7" width="17.3984375" customWidth="1"/>
     <col min="8" max="8" width="47.796875" customWidth="1"/>
-    <col min="9" max="9" width="33.3984375" style="51" customWidth="1"/>
+    <col min="9" max="9" width="33.3984375" style="44" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -4058,102 +4055,106 @@
     </row>
     <row r="2" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" t="s">
         <v>105</v>
       </c>
-      <c r="C2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="F2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I2" s="51" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="18" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="20">
+    </row>
+    <row r="3" spans="1:9" s="17" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="19">
         <v>1</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="22">
+      <c r="D3" s="97"/>
+      <c r="E3" s="21">
         <v>35</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="19">
         <v>1</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="20">
         <v>35</v>
       </c>
-      <c r="H3" s="83" t="s">
-        <v>143</v>
-      </c>
-      <c r="I3" s="52"/>
-    </row>
-    <row r="4" spans="1:9" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="19">
+      <c r="H3" s="61" t="s">
+        <v>136</v>
+      </c>
+      <c r="I3" s="45" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="18">
         <v>2</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="67"/>
-      <c r="E4" s="16">
+      <c r="D4" s="86"/>
+      <c r="E4" s="15">
         <v>9.89</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <v>1</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="15">
         <v>9.89</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="52"/>
-    </row>
-    <row r="5" spans="1:9" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="19">
+      <c r="I4" s="45" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="18">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="67"/>
-      <c r="E5" s="16">
+      <c r="D5" s="86"/>
+      <c r="E5" s="15">
         <v>60</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="16">
         <v>1</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="15">
         <v>60</v>
       </c>
-      <c r="H5" s="62" t="s">
-        <v>143</v>
-      </c>
-      <c r="I5" s="52" t="s">
-        <v>145</v>
+      <c r="H5" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="I5" s="45" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.15">
@@ -4163,10 +4164,10 @@
       <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="68" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="69"/>
+      <c r="C6" s="83" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="84"/>
       <c r="E6" s="7">
         <v>1.54</v>
       </c>
@@ -4180,91 +4181,99 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:9" s="17" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="67" t="s">
+      <c r="C7" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="67"/>
-      <c r="E7" s="16">
+      <c r="D7" s="86"/>
+      <c r="E7" s="15">
         <v>18.5</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="16">
         <v>1</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="13">
         <v>18.5</v>
       </c>
-      <c r="H7" s="84" t="s">
-        <v>143</v>
-      </c>
-      <c r="I7" s="52"/>
-    </row>
-    <row r="8" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="3">
+      <c r="H7" s="62" t="s">
+        <v>136</v>
+      </c>
+      <c r="I7" s="45" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="70">
         <v>6</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="C8" s="68" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="69"/>
-      <c r="E8" s="7">
+      <c r="B8" s="71" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="86"/>
+      <c r="E8" s="15">
         <v>42</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="16">
         <v>2</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="15">
         <v>84</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="3">
+      <c r="H8" s="69" t="s">
+        <v>140</v>
+      </c>
+      <c r="I8" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="65">
         <v>7</v>
       </c>
-      <c r="B9" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="68" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="69"/>
-      <c r="E9" s="7">
+      <c r="B9" s="63" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="85" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="86"/>
+      <c r="E9" s="15">
         <v>36.299999999999997</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="16">
         <v>2</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="15">
         <v>72.599999999999994</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="64" t="s">
         <v>13</v>
+      </c>
+      <c r="I9" s="45" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="68" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="69"/>
-      <c r="E10" s="61">
+      <c r="B10" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="83" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="84"/>
+      <c r="E10" s="53">
         <v>65</v>
       </c>
       <c r="F10" s="9">
@@ -4276,948 +4285,996 @@
       <c r="H10" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="3">
+      <c r="I10" s="44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="60">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="70">
+      <c r="C11" s="89">
         <v>237825</v>
       </c>
-      <c r="D11" s="70"/>
-      <c r="E11" s="7">
+      <c r="D11" s="89"/>
+      <c r="E11" s="15">
         <v>9.9499999999999993</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="16">
         <v>1</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="15">
         <v>9.9499999999999993</v>
       </c>
-      <c r="H11" s="23" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="30">
+      <c r="H11" s="59" t="s">
+        <v>95</v>
+      </c>
+      <c r="I11" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="28">
         <v>10</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="71" t="s">
-        <v>99</v>
-      </c>
-      <c r="D12" s="67"/>
-      <c r="E12" s="63" t="s">
+      <c r="C12" s="85" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="86"/>
+      <c r="E12" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="31">
+      <c r="F12" s="29">
         <v>1</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="14">
         <v>14.95</v>
       </c>
-      <c r="H12" s="62" t="s">
+      <c r="H12" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="I12" s="45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="28">
+        <v>11</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="86" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="86"/>
+      <c r="E13" s="15">
+        <v>25</v>
+      </c>
+      <c r="F13" s="29">
+        <v>1</v>
+      </c>
+      <c r="G13" s="13">
+        <v>25</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="45"/>
+    </row>
+    <row r="14" spans="1:9" s="80" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="74">
+        <v>12</v>
+      </c>
+      <c r="B14" s="75" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="93" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="94"/>
+      <c r="E14" s="76">
+        <v>32.869999999999997</v>
+      </c>
+      <c r="F14" s="77">
+        <v>2</v>
+      </c>
+      <c r="G14" s="78">
+        <v>65.739999999999995</v>
+      </c>
+      <c r="H14" s="78" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="79"/>
+    </row>
+    <row r="15" spans="1:9" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="28">
+        <v>13</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="85" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="86"/>
+      <c r="E15" s="15">
+        <v>10.68</v>
+      </c>
+      <c r="F15" s="16">
+        <v>2</v>
+      </c>
+      <c r="G15" s="15">
+        <v>21.36</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="28">
+        <v>14</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="86"/>
+      <c r="E16" s="55">
+        <v>5.62</v>
+      </c>
+      <c r="F16" s="16">
+        <v>2</v>
+      </c>
+      <c r="G16" s="15">
+        <v>11.24</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="33" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="95" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="96"/>
+      <c r="E17" s="56">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F17" s="32">
+        <v>1</v>
+      </c>
+      <c r="G17" s="31">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="47"/>
+    </row>
+    <row r="18" spans="1:13" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="28">
+        <v>16</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="86" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="86"/>
+      <c r="E18" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18" s="16">
+        <v>4</v>
+      </c>
+      <c r="G18" s="15">
+        <v>2.08</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="28">
+        <v>17</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="85" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="86"/>
+      <c r="E19" s="15">
+        <v>0.11</v>
+      </c>
+      <c r="F19" s="16">
+        <v>2</v>
+      </c>
+      <c r="G19" s="15">
+        <v>0.22</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="27" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="23">
+        <v>18</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="91" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="92"/>
+      <c r="E20" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="F20" s="26">
+        <v>2</v>
+      </c>
+      <c r="G20" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="46"/>
+    </row>
+    <row r="21" spans="1:13" s="27" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="23">
+        <v>19</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="91" t="s">
         <v>144</v>
       </c>
-      <c r="I12" s="52" t="s">
+      <c r="D21" s="92"/>
+      <c r="E21" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F21" s="35">
+        <v>1</v>
+      </c>
+      <c r="G21" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="46"/>
+    </row>
+    <row r="22" spans="1:13" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="18">
+        <v>20</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="85" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="86"/>
+      <c r="E22" s="15">
+        <v>1.25</v>
+      </c>
+      <c r="F22" s="16">
+        <v>1</v>
+      </c>
+      <c r="G22" s="14">
+        <v>1.25</v>
+      </c>
+      <c r="H22" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="I22" s="45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="18">
+        <v>21</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="89">
+        <v>856</v>
+      </c>
+      <c r="D23" s="89"/>
+      <c r="E23" s="55">
+        <v>3.75</v>
+      </c>
+      <c r="F23" s="29">
+        <v>1</v>
+      </c>
+      <c r="G23" s="14">
+        <v>3.75</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" s="45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="18">
+        <v>22</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="85" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="86"/>
+      <c r="E24" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="F24" s="29">
+        <v>1</v>
+      </c>
+      <c r="G24" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="18">
+        <v>23</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="89">
+        <v>2222</v>
+      </c>
+      <c r="D25" s="89"/>
+      <c r="E25" s="15">
+        <v>1</v>
+      </c>
+      <c r="F25" s="29">
+        <v>1</v>
+      </c>
+      <c r="G25" s="36">
+        <v>1</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25" s="45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="18">
+        <v>24</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="85" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="86"/>
+      <c r="E26" s="15">
+        <v>0.09</v>
+      </c>
+      <c r="F26" s="16">
+        <v>2</v>
+      </c>
+      <c r="G26" s="15">
+        <v>0.18</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" s="45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="65">
+        <v>25</v>
+      </c>
+      <c r="B27" s="63" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" s="18" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="30">
-        <v>11</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="67" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="67"/>
-      <c r="E13" s="16">
-        <v>25</v>
-      </c>
-      <c r="F13" s="31">
+      <c r="C27" s="85" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" s="86"/>
+      <c r="E27" s="15">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F27" s="16">
+        <v>4</v>
+      </c>
+      <c r="G27" s="36">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H27" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="I27" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="J27" s="73" t="s">
+        <v>135</v>
+      </c>
+      <c r="M27" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="65">
+        <v>26</v>
+      </c>
+      <c r="B28" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="85" t="s">
+        <v>128</v>
+      </c>
+      <c r="D28" s="86"/>
+      <c r="E28" s="15">
+        <v>0.79</v>
+      </c>
+      <c r="F28" s="29">
         <v>1</v>
       </c>
-      <c r="G13" s="14">
-        <v>25</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" s="52"/>
-    </row>
-    <row r="14" spans="1:9" s="29" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="24">
-        <v>12</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="72" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="73"/>
-      <c r="E14" s="27">
-        <v>32.869999999999997</v>
-      </c>
-      <c r="F14" s="28">
-        <v>2</v>
-      </c>
-      <c r="G14" s="25">
-        <v>65.739999999999995</v>
-      </c>
-      <c r="H14" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="53"/>
-    </row>
-    <row r="15" spans="1:9" s="18" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="30">
-        <v>13</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="D15" s="67"/>
-      <c r="E15" s="16">
-        <v>10.68</v>
-      </c>
-      <c r="F15" s="17">
-        <v>2</v>
-      </c>
-      <c r="G15" s="16">
-        <v>21.36</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="30">
-        <v>14</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="71" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="67"/>
-      <c r="E16" s="63">
-        <v>5.62</v>
-      </c>
-      <c r="F16" s="17">
-        <v>2</v>
-      </c>
-      <c r="G16" s="16">
-        <v>11.24</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16" s="52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="36" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="34" t="s">
+      <c r="G28" s="15">
+        <v>0.79</v>
+      </c>
+      <c r="H28" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="I28" s="72" t="s">
+        <v>132</v>
+      </c>
+      <c r="J28" s="73" t="s">
+        <v>133</v>
+      </c>
+      <c r="M28" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="60">
         <v>27</v>
       </c>
-      <c r="C17" s="74" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="75"/>
-      <c r="E17" s="64">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="F17" s="35">
+      <c r="B29" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="85">
+        <v>1952370</v>
+      </c>
+      <c r="D29" s="86"/>
+      <c r="E29" s="58">
+        <v>18.95</v>
+      </c>
+      <c r="F29" s="29">
         <v>1</v>
       </c>
-      <c r="G17" s="34">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="H17" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="54"/>
-    </row>
-    <row r="18" spans="1:10" s="18" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="30">
+      <c r="G29" s="15">
+        <v>18.95</v>
+      </c>
+      <c r="H29" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="I29" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="40" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="37">
         <v>28</v>
       </c>
-      <c r="C18" s="67" t="s">
+      <c r="B30" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="82" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="82"/>
+      <c r="E30" s="42">
+        <v>0.43</v>
+      </c>
+      <c r="F30" s="42">
+        <v>21.13</v>
+      </c>
+      <c r="G30" s="42">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="H30" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="I30" s="48"/>
+    </row>
+    <row r="31" spans="1:13" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="65">
         <v>29</v>
       </c>
-      <c r="D18" s="67"/>
-      <c r="E18" s="63" t="s">
-        <v>146</v>
-      </c>
-      <c r="F18" s="17">
-        <v>4</v>
-      </c>
-      <c r="G18" s="16">
-        <v>2.08</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="30">
-        <v>17</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="71" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="16">
-        <v>0.11</v>
-      </c>
-      <c r="F19" s="17">
-        <v>2</v>
-      </c>
-      <c r="G19" s="16">
-        <v>0.22</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" s="52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="29" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="24">
-        <v>18</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="72" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" s="73"/>
-      <c r="E20" s="27">
-        <v>0.25</v>
-      </c>
-      <c r="F20" s="28">
-        <v>2</v>
-      </c>
-      <c r="G20" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="H20" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" s="53"/>
-    </row>
-    <row r="21" spans="1:10" s="29" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="24">
-        <v>19</v>
-      </c>
-      <c r="B21" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="72" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" s="73"/>
-      <c r="E21" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="F21" s="38">
+      <c r="B31" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="85" t="s">
+        <v>127</v>
+      </c>
+      <c r="D31" s="86"/>
+      <c r="E31" s="15">
+        <v>1.28</v>
+      </c>
+      <c r="F31" s="29">
         <v>1</v>
       </c>
-      <c r="G21" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="H21" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I21" s="53"/>
-    </row>
-    <row r="22" spans="1:10" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="19">
-        <v>20</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="71" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" s="67"/>
-      <c r="E22" s="16">
-        <v>1.25</v>
-      </c>
-      <c r="F22" s="17">
-        <v>1</v>
-      </c>
-      <c r="G22" s="15">
-        <v>1.25</v>
-      </c>
-      <c r="H22" s="62" t="s">
-        <v>144</v>
-      </c>
-      <c r="I22" s="52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="18" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="19">
-        <v>21</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="76">
-        <v>856</v>
-      </c>
-      <c r="D23" s="76"/>
-      <c r="E23" s="63">
-        <v>3.75</v>
-      </c>
-      <c r="F23" s="31">
-        <v>1</v>
-      </c>
-      <c r="G23" s="15">
-        <v>3.75</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" s="52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="19">
-        <v>22</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="71" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="67"/>
-      <c r="E24" s="16">
-        <v>0.15</v>
-      </c>
-      <c r="F24" s="31">
-        <v>1</v>
-      </c>
-      <c r="G24" s="16">
-        <v>0.15</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I24" s="52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="19">
-        <v>23</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="76">
-        <v>2222</v>
-      </c>
-      <c r="D25" s="76"/>
-      <c r="E25" s="16">
-        <v>1</v>
-      </c>
-      <c r="F25" s="31">
-        <v>1</v>
-      </c>
-      <c r="G25" s="39">
-        <v>1</v>
-      </c>
-      <c r="H25" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" s="52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="18" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="19">
-        <v>24</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="D26" s="67"/>
-      <c r="E26" s="16">
-        <v>0.09</v>
-      </c>
-      <c r="F26" s="17">
-        <v>2</v>
-      </c>
-      <c r="G26" s="16">
-        <v>0.18</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I26" s="52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="3">
-        <v>25</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="68" t="s">
-        <v>136</v>
-      </c>
-      <c r="D27" s="69"/>
-      <c r="E27" s="7">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="F27" s="6">
-        <v>4</v>
-      </c>
-      <c r="G27" s="8">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I27" s="57" t="s">
-        <v>141</v>
-      </c>
-      <c r="J27" s="50" t="s">
+      <c r="G31" s="36">
+        <v>1.28</v>
+      </c>
+      <c r="H31" s="63" t="s">
+        <v>126</v>
+      </c>
+      <c r="I31" s="72" t="s">
+        <v>130</v>
+      </c>
+      <c r="J31" s="73" t="s">
+        <v>131</v>
+      </c>
+      <c r="M31" s="45" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="3">
-        <v>26</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="68" t="s">
-        <v>135</v>
-      </c>
-      <c r="D28" s="69"/>
-      <c r="E28" s="7">
-        <v>0.79</v>
-      </c>
-      <c r="F28" s="9">
-        <v>1</v>
-      </c>
-      <c r="G28" s="7">
-        <v>0.79</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I28" s="57" t="s">
-        <v>139</v>
-      </c>
-      <c r="J28" s="50" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="3">
-        <v>27</v>
-      </c>
-      <c r="B29" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="68">
-        <v>1952370</v>
-      </c>
-      <c r="D29" s="69"/>
-      <c r="E29" s="61">
-        <v>18.95</v>
-      </c>
-      <c r="F29" s="9">
-        <v>1</v>
-      </c>
-      <c r="G29" s="7">
-        <v>18.95</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="46" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="42">
-        <v>28</v>
-      </c>
-      <c r="B30" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="77" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="77"/>
-      <c r="E30" s="49">
-        <v>0.43</v>
-      </c>
-      <c r="F30" s="49">
-        <v>21.13</v>
-      </c>
-      <c r="G30" s="49">
-        <v>9.1199999999999992</v>
-      </c>
-      <c r="H30" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="I30" s="55"/>
-    </row>
-    <row r="31" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="3">
-        <v>29</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="68" t="s">
-        <v>134</v>
-      </c>
-      <c r="D31" s="69"/>
-      <c r="E31" s="7">
-        <v>1.28</v>
-      </c>
-      <c r="F31" s="9">
-        <v>1</v>
-      </c>
-      <c r="G31" s="8">
-        <v>1.28</v>
-      </c>
-      <c r="H31" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="I31" s="57" t="s">
-        <v>137</v>
-      </c>
-      <c r="J31" s="50" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="65"/>
-      <c r="B32" s="61"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="61"/>
+    <row r="32" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="57"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="53"/>
       <c r="E32" s="7"/>
       <c r="F32" s="9"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="60"/>
-      <c r="I32" s="57"/>
-      <c r="J32" s="50"/>
-    </row>
-    <row r="33" spans="1:9" s="18" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="15" t="s">
+      <c r="H32" s="52"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="43"/>
+    </row>
+    <row r="33" spans="1:10" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="14">
+        <v>29.5</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="85" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="86"/>
+      <c r="E33" s="55">
+        <v>1.25</v>
+      </c>
+      <c r="F33" s="16">
+        <v>1</v>
+      </c>
+      <c r="G33" s="36">
+        <v>1.25</v>
+      </c>
+      <c r="H33" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="I33" s="45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="60">
+        <v>30</v>
+      </c>
+      <c r="B34" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="89">
+        <v>2094346</v>
+      </c>
+      <c r="D34" s="89"/>
+      <c r="E34" s="66">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="F34" s="16">
+        <v>8</v>
+      </c>
+      <c r="G34" s="66">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="H34" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="C33" s="71" t="s">
-        <v>95</v>
-      </c>
-      <c r="D33" s="67"/>
-      <c r="E33" s="63" t="s">
+      <c r="I34" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="60">
+        <v>31</v>
+      </c>
+      <c r="B35" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="F33" s="17">
-        <v>1</v>
-      </c>
-      <c r="G33" s="39">
-        <v>1.25</v>
-      </c>
-      <c r="H33" s="62" t="s">
-        <v>144</v>
-      </c>
-      <c r="I33" s="52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="46" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="42">
-        <v>30</v>
-      </c>
-      <c r="B34" s="43" t="s">
+      <c r="C35" s="89">
+        <v>106797</v>
+      </c>
+      <c r="D35" s="89"/>
+      <c r="E35" s="66">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="F35" s="16">
+        <v>4</v>
+      </c>
+      <c r="G35" s="66">
+        <v>0.316</v>
+      </c>
+      <c r="H35" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="60">
+        <v>32</v>
+      </c>
+      <c r="B36" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="78">
-        <v>2094346</v>
-      </c>
-      <c r="D34" s="78"/>
-      <c r="E34" s="44">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="F34" s="45">
+      <c r="C36" s="90">
+        <v>106810</v>
+      </c>
+      <c r="D36" s="90"/>
+      <c r="E36" s="66">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="F36" s="16">
         <v>8</v>
       </c>
-      <c r="G34" s="44">
-        <v>0.55200000000000005</v>
-      </c>
-      <c r="H34" s="43" t="s">
+      <c r="G36" s="66">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="H36" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="I36" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="60">
+        <v>33</v>
+      </c>
+      <c r="B37" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="I34" s="55"/>
-    </row>
-    <row r="35" spans="1:9" s="46" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="42">
-        <v>31</v>
-      </c>
-      <c r="B35" s="43" t="s">
+      <c r="C37" s="89">
+        <v>38173</v>
+      </c>
+      <c r="D37" s="89"/>
+      <c r="E37" s="66">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="F37" s="16">
+        <v>4</v>
+      </c>
+      <c r="G37" s="66">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="H37" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="60">
+        <v>34</v>
+      </c>
+      <c r="B38" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="78">
-        <v>106797</v>
-      </c>
-      <c r="D35" s="78"/>
-      <c r="E35" s="44">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="F35" s="45">
+      <c r="C38" s="86">
+        <v>51553</v>
+      </c>
+      <c r="D38" s="86"/>
+      <c r="E38" s="66">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F38" s="16">
         <v>4</v>
       </c>
-      <c r="G35" s="44">
-        <v>0.316</v>
-      </c>
-      <c r="H35" s="43" t="s">
+      <c r="G38" s="66">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="H38" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="I35" s="55"/>
-    </row>
-    <row r="36" spans="1:9" s="46" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="42">
-        <v>32</v>
-      </c>
-      <c r="B36" s="43" t="s">
+      <c r="I38" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="60">
+        <v>35</v>
+      </c>
+      <c r="B39" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="79">
-        <v>106810</v>
-      </c>
-      <c r="D36" s="79"/>
-      <c r="E36" s="44">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="F36" s="45">
+      <c r="C39" s="89">
+        <v>40943</v>
+      </c>
+      <c r="D39" s="89"/>
+      <c r="E39" s="58">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F39" s="16">
+        <v>4</v>
+      </c>
+      <c r="G39" s="66">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="H39" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="60">
+        <v>36</v>
+      </c>
+      <c r="B40" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="86">
+        <v>38165</v>
+      </c>
+      <c r="D40" s="86"/>
+      <c r="E40" s="58">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F40" s="16">
+        <v>4</v>
+      </c>
+      <c r="G40" s="66">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="H40" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="60">
+        <v>37</v>
+      </c>
+      <c r="B41" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="90">
+        <v>106850</v>
+      </c>
+      <c r="D41" s="90"/>
+      <c r="E41" s="66">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F41" s="16">
+        <v>2</v>
+      </c>
+      <c r="G41" s="66">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="H41" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="I41" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="68">
+        <v>38</v>
+      </c>
+      <c r="B42" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="89">
+        <v>106826</v>
+      </c>
+      <c r="D42" s="89"/>
+      <c r="E42" s="58">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="F42" s="16">
+        <v>2</v>
+      </c>
+      <c r="G42" s="15">
+        <v>0.13</v>
+      </c>
+      <c r="H42" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="70">
+        <v>39</v>
+      </c>
+      <c r="B43" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="85" t="s">
+        <v>111</v>
+      </c>
+      <c r="D43" s="86"/>
+      <c r="E43" s="15">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F43" s="16">
+        <v>4</v>
+      </c>
+      <c r="G43" s="98">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="H43" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="I43" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="J43" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="70">
+        <v>40</v>
+      </c>
+      <c r="B44" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="85" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44" s="86"/>
+      <c r="E44" s="15">
+        <v>0.61</v>
+      </c>
+      <c r="F44" s="16">
         <v>8</v>
       </c>
-      <c r="G36" s="44">
-        <v>0.63200000000000001</v>
-      </c>
-      <c r="H36" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="I36" s="55"/>
-    </row>
-    <row r="37" spans="1:9" s="46" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="42">
-        <v>33</v>
-      </c>
-      <c r="B37" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="78">
-        <v>38173</v>
-      </c>
-      <c r="D37" s="78"/>
-      <c r="E37" s="44">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="F37" s="45">
+      <c r="G44" s="15">
+        <v>4.88</v>
+      </c>
+      <c r="H44" s="71" t="s">
+        <v>147</v>
+      </c>
+      <c r="I44" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="J44" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="70">
+        <v>41</v>
+      </c>
+      <c r="B45" s="69" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="85" t="s">
+        <v>110</v>
+      </c>
+      <c r="D45" s="86"/>
+      <c r="E45" s="15">
+        <v>0.54</v>
+      </c>
+      <c r="F45" s="16">
         <v>4</v>
       </c>
-      <c r="G37" s="44">
-        <v>0.39600000000000002</v>
-      </c>
-      <c r="H37" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="I37" s="55"/>
-    </row>
-    <row r="38" spans="1:9" s="46" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="42">
-        <v>34</v>
-      </c>
-      <c r="B38" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38" s="77">
-        <v>51553</v>
-      </c>
-      <c r="D38" s="77"/>
-      <c r="E38" s="44">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="F38" s="45">
-        <v>4</v>
-      </c>
-      <c r="G38" s="44">
-        <v>0.23599999999999999</v>
-      </c>
-      <c r="H38" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="55"/>
-    </row>
-    <row r="39" spans="1:9" s="46" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="42">
-        <v>35</v>
-      </c>
-      <c r="B39" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" s="78">
-        <v>40943</v>
-      </c>
-      <c r="D39" s="78"/>
-      <c r="E39" s="59">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="F39" s="45">
-        <v>4</v>
-      </c>
-      <c r="G39" s="44">
-        <v>0.23599999999999999</v>
-      </c>
-      <c r="H39" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" s="55"/>
-    </row>
-    <row r="40" spans="1:9" s="46" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="42">
-        <v>36</v>
-      </c>
-      <c r="B40" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="C40" s="77">
-        <v>38165</v>
-      </c>
-      <c r="D40" s="77"/>
-      <c r="E40" s="59">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="F40" s="45">
-        <v>4</v>
-      </c>
-      <c r="G40" s="44">
-        <v>0.23599999999999999</v>
-      </c>
-      <c r="H40" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" s="55"/>
-    </row>
-    <row r="41" spans="1:9" s="46" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="42">
-        <v>37</v>
-      </c>
-      <c r="B41" s="47" t="s">
+      <c r="G45" s="98">
+        <v>2.16</v>
+      </c>
+      <c r="H45" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="79">
-        <v>106850</v>
-      </c>
-      <c r="D41" s="79"/>
-      <c r="E41" s="44">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="F41" s="45">
+      <c r="I45" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="J45" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="70">
+        <v>42</v>
+      </c>
+      <c r="B46" s="69" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" s="85" t="s">
+        <v>109</v>
+      </c>
+      <c r="D46" s="86"/>
+      <c r="E46" s="15">
+        <v>0.27</v>
+      </c>
+      <c r="F46" s="16">
         <v>2</v>
       </c>
-      <c r="G41" s="44">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="H41" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="I41" s="55"/>
-    </row>
-    <row r="42" spans="1:9" s="46" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="48">
-        <v>38</v>
-      </c>
-      <c r="B42" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" s="78">
-        <v>106826</v>
-      </c>
-      <c r="D42" s="78"/>
-      <c r="E42" s="59">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="F42" s="45">
-        <v>2</v>
-      </c>
-      <c r="G42" s="49">
-        <v>0.13</v>
-      </c>
-      <c r="H42" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" s="55"/>
-    </row>
-    <row r="43" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="3">
-        <v>39</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C43" s="68" t="s">
-        <v>117</v>
-      </c>
-      <c r="D43" s="69"/>
-      <c r="E43" s="7">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F43" s="6">
-        <v>4</v>
-      </c>
-      <c r="G43" s="12">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I43" s="51" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="3">
-        <v>40</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" s="68" t="s">
-        <v>114</v>
-      </c>
-      <c r="D44" s="69"/>
-      <c r="E44" s="7">
-        <v>0.61</v>
-      </c>
-      <c r="F44" s="6">
-        <v>8</v>
-      </c>
-      <c r="G44" s="7">
-        <v>4.88</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I44" s="51" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="3">
-        <v>41</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C45" s="68" t="s">
-        <v>116</v>
-      </c>
-      <c r="D45" s="69"/>
-      <c r="E45" s="7">
+      <c r="G46" s="15">
         <v>0.54</v>
       </c>
-      <c r="F45" s="6">
-        <v>4</v>
-      </c>
-      <c r="G45" s="12">
-        <v>2.16</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I45" s="51" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="3">
-        <v>42</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" s="68" t="s">
+      <c r="H46" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="I46" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="D46" s="69"/>
-      <c r="E46" s="7">
-        <v>0.27</v>
-      </c>
-      <c r="F46" s="6">
-        <v>2</v>
-      </c>
-      <c r="G46" s="7">
-        <v>0.54</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I46" s="51" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J46" s="45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3">
         <v>43</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" s="69" t="s">
-        <v>124</v>
-      </c>
-      <c r="D47" s="69"/>
+        <v>59</v>
+      </c>
+      <c r="C47" s="84" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47" s="84"/>
       <c r="E47" s="11">
         <v>0.41799999999999998</v>
       </c>
@@ -5228,23 +5285,26 @@
         <v>0.83599999999999997</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="I47" s="51" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+        <v>116</v>
+      </c>
+      <c r="I47" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="J47" s="43" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3">
         <v>44</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C48" s="80" t="s">
-        <v>126</v>
-      </c>
-      <c r="D48" s="69"/>
+        <v>60</v>
+      </c>
+      <c r="C48" s="87" t="s">
+        <v>120</v>
+      </c>
+      <c r="D48" s="84"/>
       <c r="E48" s="11">
         <v>0.246</v>
       </c>
@@ -5255,10 +5315,10 @@
         <v>0.98399999999999999</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="I48" s="51" t="s">
-        <v>127</v>
+        <v>117</v>
+      </c>
+      <c r="I48" s="44" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -5266,12 +5326,12 @@
         <v>45</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C49" s="68" t="s">
-        <v>128</v>
-      </c>
-      <c r="D49" s="69"/>
+        <v>61</v>
+      </c>
+      <c r="C49" s="83" t="s">
+        <v>122</v>
+      </c>
+      <c r="D49" s="84"/>
       <c r="E49" s="11">
         <v>0.246</v>
       </c>
@@ -5279,40 +5339,40 @@
         <v>21</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H49" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="I49" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="I49" s="51" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" s="46" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="42">
+    </row>
+    <row r="50" spans="1:9" s="17" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="60">
         <v>46</v>
       </c>
-      <c r="B50" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C50" s="82">
+      <c r="B50" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" s="85">
         <v>2135064</v>
       </c>
-      <c r="D50" s="77"/>
-      <c r="E50" s="49">
+      <c r="D50" s="86"/>
+      <c r="E50" s="15">
         <v>2.4900000000000002</v>
       </c>
-      <c r="F50" s="45">
+      <c r="F50" s="16">
         <v>2</v>
       </c>
-      <c r="G50" s="49">
+      <c r="G50" s="15">
         <v>4.9800000000000004</v>
       </c>
-      <c r="H50" s="43" t="s">
+      <c r="H50" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="I50" s="55" t="s">
-        <v>113</v>
+      <c r="I50" s="45" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -5320,13 +5380,13 @@
         <v>47</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C51" s="80" t="s">
-        <v>101</v>
-      </c>
-      <c r="D51" s="69"/>
-      <c r="E51" s="65">
+        <v>64</v>
+      </c>
+      <c r="C51" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="D51" s="84"/>
+      <c r="E51" s="57">
         <v>67</v>
       </c>
       <c r="F51" s="5">
@@ -5336,123 +5396,171 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" s="46" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="56">
+        <v>65</v>
+      </c>
+      <c r="I51" s="44" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="40" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="49">
         <v>48</v>
       </c>
-      <c r="B52" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="C52" s="82" t="s">
-        <v>103</v>
-      </c>
-      <c r="D52" s="77"/>
-      <c r="E52" s="49">
+      <c r="B52" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="88" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" s="82"/>
+      <c r="E52" s="42">
         <v>9.99</v>
       </c>
-      <c r="F52" s="45">
+      <c r="F52" s="39">
         <v>1</v>
       </c>
-      <c r="G52" s="49">
+      <c r="G52" s="42">
         <v>9.99</v>
       </c>
-      <c r="H52" s="43" t="s">
+      <c r="H52" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="I52" s="55"/>
+      <c r="I52" s="48"/>
     </row>
     <row r="53" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="3">
         <v>49</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C53" s="68" t="s">
-        <v>131</v>
-      </c>
-      <c r="D53" s="69"/>
+        <v>124</v>
+      </c>
+      <c r="C53" s="83" t="s">
+        <v>125</v>
+      </c>
+      <c r="D53" s="84"/>
       <c r="E53" s="10"/>
       <c r="F53" s="6">
         <v>5</v>
       </c>
       <c r="G53" s="10"/>
       <c r="H53" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I53" s="44" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="40" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="37">
+        <v>50</v>
+      </c>
+      <c r="B54" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="81" t="s">
+        <v>99</v>
+      </c>
+      <c r="D54" s="82"/>
+      <c r="E54" s="41"/>
+      <c r="F54" s="51">
+        <v>5</v>
+      </c>
+      <c r="G54" s="41"/>
+      <c r="H54" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="I54" s="48"/>
+    </row>
+    <row r="55" spans="1:9" s="40" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="37">
+        <v>51</v>
+      </c>
+      <c r="B55" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="I53" s="51" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" s="46" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="42">
-        <v>50</v>
-      </c>
-      <c r="B54" s="43" t="s">
+      <c r="D55" s="82"/>
+      <c r="E55" s="41"/>
+      <c r="F55" s="41"/>
+      <c r="G55" s="41"/>
+      <c r="H55" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C54" s="81" t="s">
-        <v>104</v>
-      </c>
-      <c r="D54" s="77"/>
-      <c r="E54" s="47"/>
-      <c r="F54" s="58">
-        <v>5</v>
-      </c>
-      <c r="G54" s="47"/>
-      <c r="H54" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="I54" s="55"/>
-    </row>
-    <row r="55" spans="1:9" s="46" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="42">
-        <v>51</v>
-      </c>
-      <c r="B55" s="47" t="s">
+      <c r="I55" s="48"/>
+    </row>
+    <row r="56" spans="1:9" s="40" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="C55" s="77" t="s">
+      <c r="B56" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="D55" s="77"/>
-      <c r="E55" s="47"/>
-      <c r="F55" s="47"/>
-      <c r="G55" s="47"/>
-      <c r="H55" s="43" t="s">
+      <c r="C56" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="I55" s="55"/>
-    </row>
-    <row r="56" spans="1:9" s="46" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="43" t="s">
+      <c r="D56" s="82"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="41"/>
+      <c r="H56" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="B56" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="C56" s="77" t="s">
-        <v>77</v>
-      </c>
-      <c r="D56" s="77"/>
-      <c r="E56" s="47"/>
-      <c r="F56" s="47"/>
-      <c r="G56" s="47"/>
-      <c r="H56" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="I56" s="55"/>
+      <c r="I56" s="48"/>
     </row>
     <row r="57" spans="1:9" ht="83" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
     <mergeCell ref="C54:D54"/>
     <mergeCell ref="C55:D55"/>
     <mergeCell ref="C56:D56"/>
@@ -5461,51 +5569,6 @@
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I31" r:id="rId1" xr:uid="{A02AF87C-9527-A047-9DFE-4A7472C1BB6D}"/>

</xml_diff>

<commit_message>
update of folders and syringe pump
</commit_message>
<xml_diff>
--- a/Minidrop build and test/Our aid documents and purchases/BOM.xlsx
+++ b/Minidrop build and test/Our aid documents and purchases/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twenzel/Documents/GitHub/OpenMicrofluidics/Minidrop build and test/Our aid documents and purchases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D14EF84-89E0-5D4B-9EF7-1474D84CB30C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24934801-8545-DC4C-A9F2-1937FE4573F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2680" yWindow="-18840" windowWidth="20120" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34360" yWindow="-1420" windowWidth="20120" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -593,109 +593,109 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1572,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.3984375" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -1613,1230 +1613,1230 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="9" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="37">
+    <row r="3" spans="1:10" s="8" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="31">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7">
+      <c r="D3" s="35"/>
+      <c r="E3" s="6">
         <v>35</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
       </c>
-      <c r="G3" s="40">
+      <c r="G3" s="34">
         <v>35</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="14">
+    <row r="4" spans="1:10" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="12">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12">
+      <c r="D4" s="36"/>
+      <c r="E4" s="10">
         <v>9.89</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="11">
         <v>1</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="10">
         <v>9.89</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="9" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="14">
+    <row r="5" spans="1:10" s="8" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="12">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12">
+      <c r="D5" s="36"/>
+      <c r="E5" s="10">
         <v>60</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="11">
         <v>1</v>
       </c>
-      <c r="G5" s="39">
+      <c r="G5" s="33">
         <v>60</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="9" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="14">
+    <row r="6" spans="1:10" s="8" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="12">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12">
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="10">
         <v>1.54</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="11">
         <v>1</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="10">
         <v>1.54</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="7" t="s">
         <v>140</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="9" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:10" s="8" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12">
+      <c r="D7" s="36"/>
+      <c r="E7" s="10">
         <v>18.5</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="11">
         <v>1</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="9">
         <v>18.5</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="14">
+    <row r="8" spans="1:10" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="12">
         <v>6</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12">
+      <c r="D8" s="36"/>
+      <c r="E8" s="10">
         <v>42</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="11">
         <v>2</v>
       </c>
-      <c r="G8" s="39">
+      <c r="G8" s="33">
         <v>84</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="14">
+    <row r="9" spans="1:10" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="12">
         <v>7</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12">
+      <c r="D9" s="36"/>
+      <c r="E9" s="10">
         <v>36.299999999999997</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="11">
         <v>2</v>
       </c>
-      <c r="G9" s="39">
+      <c r="G9" s="33">
         <v>72.599999999999994</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="14">
+    <row r="10" spans="1:10" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="12">
         <v>8</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="12">
+      <c r="D10" s="37"/>
+      <c r="E10" s="10">
         <v>65</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="11">
         <v>1</v>
       </c>
-      <c r="G10" s="39">
+      <c r="G10" s="33">
         <v>65</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="14">
+    <row r="11" spans="1:10" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="12">
         <v>9</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="37">
         <v>237825</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="12">
+      <c r="D11" s="37"/>
+      <c r="E11" s="10">
         <v>9.9499999999999993</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="11">
         <v>1</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="10">
         <v>9.9499999999999993</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="14">
+    <row r="12" spans="1:10" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="12">
         <v>10</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="10" t="s">
+      <c r="D12" s="36"/>
+      <c r="E12" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="11">
         <v>1</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="9">
         <v>14.95</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="9" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="14">
+    <row r="13" spans="1:10" s="8" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="12">
         <v>11</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12">
+      <c r="D13" s="36"/>
+      <c r="E13" s="10">
         <v>25</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="11">
         <v>1</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="9">
         <v>25</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="15">
+    <row r="14" spans="1:10" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="13">
         <v>12</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="10">
+      <c r="D14" s="36"/>
+      <c r="E14" s="9">
         <v>32.869999999999997</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="11">
         <v>2</v>
       </c>
-      <c r="G14" s="38">
+      <c r="G14" s="32">
         <v>65.739999999999995</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="9" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="14">
+    <row r="15" spans="1:10" s="8" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="12">
         <v>13</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12">
+      <c r="D15" s="36"/>
+      <c r="E15" s="10">
         <v>10.68</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="11">
         <v>2</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="10">
         <v>21.36</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="9" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="14">
+    <row r="16" spans="1:10" s="8" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="12">
         <v>14</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="10">
+      <c r="D16" s="36"/>
+      <c r="E16" s="9">
         <v>5.62</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="11">
         <v>2</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="10">
         <v>11.24</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="24" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="15">
+    <row r="17" spans="1:13" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="13">
         <v>15</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="20">
+      <c r="D17" s="38"/>
+      <c r="E17" s="16">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="18">
         <v>1</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="16">
         <v>0.56999999999999995</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="I17" s="36" t="s">
+      <c r="I17" s="30" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="9" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="14">
+    <row r="18" spans="1:13" s="8" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="12">
         <v>16</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="10" t="s">
+      <c r="D18" s="36"/>
+      <c r="E18" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="11">
         <v>4</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="10">
         <v>2.08</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I18" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="14">
+    <row r="19" spans="1:13" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="12">
         <v>17</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12">
+      <c r="D19" s="36"/>
+      <c r="E19" s="10">
         <v>0.11</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="11">
         <v>2</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="10">
         <v>0.22</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="24" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="14">
+    <row r="20" spans="1:13" s="19" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="12">
         <v>18</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="22">
+      <c r="D20" s="38"/>
+      <c r="E20" s="17">
         <v>0.25</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="18">
         <v>2</v>
       </c>
-      <c r="G20" s="22">
+      <c r="G20" s="17">
         <v>0.5</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="H20" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="I20" s="24" t="s">
+      <c r="I20" s="19" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="24" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="14">
+    <row r="21" spans="1:13" s="19" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="12">
         <v>19</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22">
+      <c r="D21" s="38"/>
+      <c r="E21" s="17">
         <v>0.1</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="18">
         <v>1</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G21" s="17">
         <v>0.1</v>
       </c>
-      <c r="H21" s="20" t="s">
+      <c r="H21" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="I21" s="24" t="s">
+      <c r="I21" s="19" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="14">
+    <row r="22" spans="1:13" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="12">
         <v>20</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12">
+      <c r="D22" s="36"/>
+      <c r="E22" s="10">
         <v>1.25</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="11">
         <v>1</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="9">
         <v>1.25</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="9" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="14">
+    <row r="23" spans="1:13" s="8" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="12">
         <v>21</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="37">
         <v>856</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="10">
+      <c r="D23" s="37"/>
+      <c r="E23" s="9">
         <v>3.75</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="11">
         <v>1</v>
       </c>
-      <c r="G23" s="10">
+      <c r="G23" s="9">
         <v>3.75</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="I23" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="14">
+    <row r="24" spans="1:13" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="12">
         <v>22</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12">
+      <c r="D24" s="36"/>
+      <c r="E24" s="10">
         <v>0.15</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="11">
         <v>1</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="10">
         <v>0.15</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="I24" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="14">
+    <row r="25" spans="1:13" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="12">
         <v>23</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="37">
         <v>2222</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="12">
+      <c r="D25" s="37"/>
+      <c r="E25" s="10">
         <v>1</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="11">
         <v>1</v>
       </c>
-      <c r="G25" s="12">
+      <c r="G25" s="10">
         <v>1</v>
       </c>
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="I25" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="9" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="14">
+    <row r="26" spans="1:13" s="8" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="12">
         <v>24</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="12">
+      <c r="D26" s="36"/>
+      <c r="E26" s="10">
         <v>0.09</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="11">
         <v>2</v>
       </c>
-      <c r="G26" s="12">
+      <c r="G26" s="10">
         <v>0.18</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="H26" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="I26" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="14">
+    <row r="27" spans="1:13" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="12">
         <v>25</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="12">
+      <c r="D27" s="36"/>
+      <c r="E27" s="10">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27" s="11">
         <v>4</v>
       </c>
-      <c r="G27" s="12">
+      <c r="G27" s="10">
         <v>1.1599999999999999</v>
       </c>
-      <c r="H27" s="10" t="s">
+      <c r="H27" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I27" s="25" t="s">
+      <c r="I27" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="J27" s="9" t="s">
+      <c r="J27" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="M27" s="8" t="s">
+      <c r="M27" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="14">
+    <row r="28" spans="1:13" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="12">
         <v>26</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="12">
+      <c r="D28" s="36"/>
+      <c r="E28" s="10">
         <v>0.79</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28" s="11">
         <v>1</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G28" s="10">
         <v>0.79</v>
       </c>
-      <c r="H28" s="10" t="s">
+      <c r="H28" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I28" s="25" t="s">
+      <c r="I28" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="J28" s="9" t="s">
+      <c r="J28" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="M28" s="8" t="s">
+      <c r="M28" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="14">
+    <row r="29" spans="1:13" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="12">
         <v>27</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="36">
         <v>1952370</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="10">
+      <c r="D29" s="36"/>
+      <c r="E29" s="9">
         <v>18.95</v>
       </c>
-      <c r="F29" s="13">
+      <c r="F29" s="11">
         <v>1</v>
       </c>
-      <c r="G29" s="12">
+      <c r="G29" s="10">
         <v>18.95</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="H29" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="I29" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="30" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="14">
+    <row r="30" spans="1:13" s="24" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="12">
         <v>28</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="28">
+      <c r="D30" s="39"/>
+      <c r="E30" s="22">
         <v>0.43</v>
       </c>
-      <c r="F30" s="28">
+      <c r="F30" s="22">
         <v>21.13</v>
       </c>
-      <c r="G30" s="28">
+      <c r="G30" s="22">
         <v>9.1199999999999992</v>
       </c>
-      <c r="H30" s="26" t="s">
+      <c r="H30" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="I30" s="29" t="s">
+      <c r="I30" s="23" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="14">
+    <row r="31" spans="1:13" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="12">
         <v>29</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="12">
+      <c r="D31" s="36"/>
+      <c r="E31" s="10">
         <v>1.28</v>
       </c>
-      <c r="F31" s="13">
+      <c r="F31" s="11">
         <v>1</v>
       </c>
-      <c r="G31" s="12">
+      <c r="G31" s="10">
         <v>1.28</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="H31" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I31" s="25" t="s">
+      <c r="I31" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="J31" s="9" t="s">
+      <c r="J31" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="M31" s="8" t="s">
+      <c r="M31" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="14"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="31"/>
-    </row>
-    <row r="33" spans="1:10" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="15">
+      <c r="A32" s="12"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="25"/>
+    </row>
+    <row r="33" spans="1:10" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="13">
         <v>30</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="10">
+      <c r="D33" s="36"/>
+      <c r="E33" s="9">
         <v>1.25</v>
       </c>
-      <c r="F33" s="13">
+      <c r="F33" s="11">
         <v>1</v>
       </c>
-      <c r="G33" s="12">
+      <c r="G33" s="10">
         <v>1.25</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="H33" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="I33" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="15">
+    <row r="34" spans="1:10" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="13">
         <v>31</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C34" s="19">
+      <c r="C34" s="37">
         <v>2094346</v>
       </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="32">
+      <c r="D34" s="37"/>
+      <c r="E34" s="26">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="F34" s="13">
+      <c r="F34" s="11">
         <v>8</v>
       </c>
-      <c r="G34" s="32">
+      <c r="G34" s="26">
         <v>0.55200000000000005</v>
       </c>
-      <c r="H34" s="10" t="s">
+      <c r="H34" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I34" s="8" t="s">
+      <c r="I34" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="9" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="15">
+    <row r="35" spans="1:10" s="8" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="13">
         <v>32</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="19">
+      <c r="C35" s="37">
         <v>106797</v>
       </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="32">
+      <c r="D35" s="37"/>
+      <c r="E35" s="26">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="F35" s="13">
+      <c r="F35" s="11">
         <v>4</v>
       </c>
-      <c r="G35" s="32">
+      <c r="G35" s="26">
         <v>0.316</v>
       </c>
-      <c r="H35" s="10" t="s">
+      <c r="H35" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I35" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="9" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="15">
+    <row r="36" spans="1:10" s="8" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="13">
         <v>33</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C36" s="37">
         <v>106810</v>
       </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="32">
+      <c r="D36" s="37"/>
+      <c r="E36" s="26">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="F36" s="13">
+      <c r="F36" s="11">
         <v>8</v>
       </c>
-      <c r="G36" s="32">
+      <c r="G36" s="26">
         <v>0.63200000000000001</v>
       </c>
-      <c r="H36" s="10" t="s">
+      <c r="H36" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I36" s="8" t="s">
+      <c r="I36" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="9" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="15">
+    <row r="37" spans="1:10" s="8" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="13">
         <v>34</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="19">
+      <c r="C37" s="37">
         <v>38173</v>
       </c>
-      <c r="D37" s="19"/>
-      <c r="E37" s="32">
+      <c r="D37" s="37"/>
+      <c r="E37" s="26">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="F37" s="13">
+      <c r="F37" s="11">
         <v>4</v>
       </c>
-      <c r="G37" s="32">
+      <c r="G37" s="26">
         <v>0.39600000000000002</v>
       </c>
-      <c r="H37" s="10" t="s">
+      <c r="H37" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I37" s="8" t="s">
+      <c r="I37" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="15">
+    <row r="38" spans="1:10" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="13">
         <v>35</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="36">
         <v>51553</v>
       </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="32">
+      <c r="D38" s="36"/>
+      <c r="E38" s="26">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="F38" s="13">
+      <c r="F38" s="11">
         <v>4</v>
       </c>
-      <c r="G38" s="32">
+      <c r="G38" s="26">
         <v>0.23599999999999999</v>
       </c>
-      <c r="H38" s="10" t="s">
+      <c r="H38" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I38" s="8" t="s">
+      <c r="I38" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="9" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="15">
+    <row r="39" spans="1:10" s="8" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="13">
         <v>36</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C39" s="19">
+      <c r="C39" s="37">
         <v>40943</v>
       </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="10">
+      <c r="D39" s="37"/>
+      <c r="E39" s="9">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="F39" s="13">
+      <c r="F39" s="11">
         <v>4</v>
       </c>
-      <c r="G39" s="32">
+      <c r="G39" s="26">
         <v>0.23599999999999999</v>
       </c>
-      <c r="H39" s="10" t="s">
+      <c r="H39" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I39" s="8" t="s">
+      <c r="I39" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="15">
+    <row r="40" spans="1:10" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="13">
         <v>37</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C40" s="36">
         <v>38165</v>
       </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="10">
+      <c r="D40" s="36"/>
+      <c r="E40" s="9">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="F40" s="13">
+      <c r="F40" s="11">
         <v>4</v>
       </c>
-      <c r="G40" s="32">
+      <c r="G40" s="26">
         <v>0.23599999999999999</v>
       </c>
-      <c r="H40" s="10" t="s">
+      <c r="H40" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I40" s="8" t="s">
+      <c r="I40" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="15">
+    <row r="41" spans="1:10" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="13">
         <v>38</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C41" s="19">
+      <c r="C41" s="37">
         <v>106850</v>
       </c>
-      <c r="D41" s="19"/>
-      <c r="E41" s="32">
+      <c r="D41" s="37"/>
+      <c r="E41" s="26">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="F41" s="13">
+      <c r="F41" s="11">
         <v>2</v>
       </c>
-      <c r="G41" s="32">
+      <c r="G41" s="26">
         <v>0.11799999999999999</v>
       </c>
-      <c r="H41" s="10" t="s">
+      <c r="H41" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I41" s="8" t="s">
+      <c r="I41" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="9" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="15">
+    <row r="42" spans="1:10" s="8" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="13">
         <v>39</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C42" s="19">
+      <c r="C42" s="37">
         <v>106826</v>
       </c>
-      <c r="D42" s="19"/>
-      <c r="E42" s="10">
+      <c r="D42" s="37"/>
+      <c r="E42" s="9">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="F42" s="13">
+      <c r="F42" s="11">
         <v>2</v>
       </c>
-      <c r="G42" s="12">
+      <c r="G42" s="10">
         <v>0.13</v>
       </c>
-      <c r="H42" s="10" t="s">
+      <c r="H42" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I42" s="8" t="s">
+      <c r="I42" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="15">
+    <row r="43" spans="1:10" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="13">
         <v>40</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D43" s="11"/>
-      <c r="E43" s="12">
+      <c r="D43" s="36"/>
+      <c r="E43" s="10">
         <v>0.56000000000000005</v>
       </c>
-      <c r="F43" s="13">
+      <c r="F43" s="11">
         <v>4</v>
       </c>
-      <c r="G43" s="12">
+      <c r="G43" s="10">
         <v>2.2400000000000002</v>
       </c>
-      <c r="H43" s="10" t="s">
+      <c r="H43" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="I43" s="8" t="s">
+      <c r="I43" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J43" s="8" t="s">
+      <c r="J43" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="15">
+    <row r="44" spans="1:10" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="13">
         <v>41</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D44" s="11"/>
-      <c r="E44" s="12">
+      <c r="D44" s="36"/>
+      <c r="E44" s="10">
         <v>0.61</v>
       </c>
-      <c r="F44" s="13">
+      <c r="F44" s="11">
         <v>8</v>
       </c>
-      <c r="G44" s="12">
+      <c r="G44" s="10">
         <v>4.88</v>
       </c>
-      <c r="H44" s="10" t="s">
+      <c r="H44" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="I44" s="8" t="s">
+      <c r="I44" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J44" s="8" t="s">
+      <c r="J44" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="9" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="15">
+    <row r="45" spans="1:10" s="8" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="13">
         <v>42</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D45" s="11"/>
-      <c r="E45" s="12">
+      <c r="D45" s="36"/>
+      <c r="E45" s="10">
         <v>0.54</v>
       </c>
-      <c r="F45" s="13">
+      <c r="F45" s="11">
         <v>4</v>
       </c>
-      <c r="G45" s="12">
+      <c r="G45" s="10">
         <v>2.16</v>
       </c>
-      <c r="H45" s="10" t="s">
+      <c r="H45" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="I45" s="8" t="s">
+      <c r="I45" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J45" s="8" t="s">
+      <c r="J45" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="15">
+    <row r="46" spans="1:10" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="13">
         <v>43</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="D46" s="11"/>
-      <c r="E46" s="12">
+      <c r="D46" s="36"/>
+      <c r="E46" s="10">
         <v>0.27</v>
       </c>
-      <c r="F46" s="13">
+      <c r="F46" s="11">
         <v>2</v>
       </c>
-      <c r="G46" s="12">
+      <c r="G46" s="10">
         <v>0.54</v>
       </c>
-      <c r="H46" s="10" t="s">
+      <c r="H46" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="I46" s="8" t="s">
+      <c r="I46" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J46" s="8" t="s">
+      <c r="J46" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="15">
+      <c r="A47" s="13">
         <v>44</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="C47" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="D47" s="16"/>
-      <c r="E47" s="33">
+      <c r="D47" s="40"/>
+      <c r="E47" s="27">
         <v>0.41799999999999998</v>
       </c>
-      <c r="F47" s="18">
+      <c r="F47" s="15">
         <v>2</v>
       </c>
-      <c r="G47" s="33">
+      <c r="G47" s="27">
         <v>0.83599999999999997</v>
       </c>
-      <c r="H47" s="15" t="s">
+      <c r="H47" s="13" t="s">
         <v>119</v>
       </c>
       <c r="I47" s="3" t="s">
@@ -2847,26 +2847,26 @@
       </c>
     </row>
     <row r="48" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="15">
+      <c r="A48" s="13">
         <v>45</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="C48" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="D48" s="16"/>
-      <c r="E48" s="33">
+      <c r="D48" s="40"/>
+      <c r="E48" s="27">
         <v>0.246</v>
       </c>
-      <c r="F48" s="18">
+      <c r="F48" s="15">
         <v>4</v>
       </c>
-      <c r="G48" s="33">
+      <c r="G48" s="27">
         <v>0.98399999999999999</v>
       </c>
-      <c r="H48" s="15" t="s">
+      <c r="H48" s="13" t="s">
         <v>119</v>
       </c>
       <c r="I48" s="3" t="s">
@@ -2874,108 +2874,108 @@
       </c>
     </row>
     <row r="49" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="15">
+      <c r="A49" s="13">
         <v>46</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="C49" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="D49" s="16"/>
-      <c r="E49" s="33">
+      <c r="D49" s="40"/>
+      <c r="E49" s="27">
         <v>0.246</v>
       </c>
-      <c r="F49" s="18">
+      <c r="F49" s="15">
         <v>21</v>
       </c>
-      <c r="G49" s="15" t="s">
+      <c r="G49" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="H49" s="15" t="s">
+      <c r="H49" s="13" t="s">
         <v>119</v>
       </c>
       <c r="I49" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="9" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="15">
+    <row r="50" spans="1:10" s="8" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="13">
         <v>47</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C50" s="11">
+      <c r="C50" s="36">
         <v>2135064</v>
       </c>
-      <c r="D50" s="11"/>
-      <c r="E50" s="12">
+      <c r="D50" s="36"/>
+      <c r="E50" s="10">
         <v>2.4900000000000002</v>
       </c>
-      <c r="F50" s="13">
+      <c r="F50" s="11">
         <v>2</v>
       </c>
-      <c r="G50" s="12">
+      <c r="G50" s="10">
         <v>4.9800000000000004</v>
       </c>
-      <c r="H50" s="10" t="s">
+      <c r="H50" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I50" s="8" t="s">
+      <c r="I50" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="15">
+      <c r="A51" s="13">
         <v>48</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="C51" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="D51" s="16"/>
-      <c r="E51" s="14">
+      <c r="D51" s="40"/>
+      <c r="E51" s="12">
         <v>67</v>
       </c>
-      <c r="F51" s="34">
+      <c r="F51" s="28">
         <v>0.06</v>
       </c>
-      <c r="G51" s="17">
+      <c r="G51" s="14">
         <v>4.0199999999999996</v>
       </c>
-      <c r="H51" s="15" t="s">
+      <c r="H51" s="13" t="s">
         <v>124</v>
       </c>
       <c r="I51" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="9" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="15">
+    <row r="52" spans="1:10" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="13">
         <v>49</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="12">
+      <c r="C52" s="36"/>
+      <c r="D52" s="36"/>
+      <c r="E52" s="10">
         <v>9.99</v>
       </c>
-      <c r="F52" s="13">
+      <c r="F52" s="11">
         <v>1</v>
       </c>
-      <c r="G52" s="12">
+      <c r="G52" s="10">
         <v>9.99</v>
       </c>
-      <c r="H52" s="10" t="s">
+      <c r="H52" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="I52" s="8" t="s">
+      <c r="I52" s="7" t="s">
         <v>143</v>
       </c>
       <c r="J52" s="1" t="s">
@@ -2983,88 +2983,88 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="15">
+      <c r="A53" s="13">
         <v>50</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C53" s="16" t="s">
+      <c r="C53" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="D53" s="16"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="18">
+      <c r="D53" s="40"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="15">
         <v>5</v>
       </c>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15" t="s">
+      <c r="G53" s="13"/>
+      <c r="H53" s="13" t="s">
         <v>125</v>
       </c>
       <c r="I53" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="30" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="15">
+    <row r="54" spans="1:10" s="24" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="13">
         <v>51</v>
       </c>
-      <c r="B54" s="26" t="s">
+      <c r="B54" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="C54" s="27" t="s">
+      <c r="C54" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D54" s="27"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="35">
+      <c r="D54" s="39"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="29">
         <v>5</v>
       </c>
-      <c r="G54" s="26"/>
-      <c r="H54" s="26" t="s">
+      <c r="G54" s="21"/>
+      <c r="H54" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="I54" s="29"/>
-    </row>
-    <row r="55" spans="1:10" s="30" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="15">
+      <c r="I54" s="23"/>
+    </row>
+    <row r="55" spans="1:10" s="24" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="13">
         <v>52</v>
       </c>
-      <c r="B55" s="26" t="s">
+      <c r="B55" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="C55" s="27" t="s">
+      <c r="C55" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="D55" s="27"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="26"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="26" t="s">
+      <c r="D55" s="39"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="I55" s="29" t="s">
+      <c r="I55" s="23" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="30" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="15">
+    <row r="56" spans="1:10" s="24" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="13">
         <v>53</v>
       </c>
-      <c r="B56" s="26" t="s">
+      <c r="B56" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="C56" s="27" t="s">
+      <c r="C56" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="D56" s="27"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="26"/>
-      <c r="G56" s="26"/>
-      <c r="H56" s="26" t="s">
+      <c r="D56" s="39"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="I56" s="29" t="s">
+      <c r="I56" s="23" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3075,51 +3075,6 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
     <mergeCell ref="C54:D54"/>
     <mergeCell ref="C55:D55"/>
     <mergeCell ref="C56:D56"/>
@@ -3128,6 +3083,51 @@
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I31" r:id="rId1" xr:uid="{A02AF87C-9527-A047-9DFE-4A7472C1BB6D}"/>

</xml_diff>

<commit_message>
add subprojects and files as well as build photos
</commit_message>
<xml_diff>
--- a/Minidrop build and test/Our aid documents and purchases/BOM.xlsx
+++ b/Minidrop build and test/Our aid documents and purchases/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twenzel/Documents/GitHub/OpenMicrofluidics/Minidrop build and test/Our aid documents and purchases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24934801-8545-DC4C-A9F2-1937FE4573F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE25159-6877-CB44-AE96-F803EF0FC128}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34360" yWindow="-1420" windowWidth="20120" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22800" yWindow="520" windowWidth="20120" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="150">
   <si>
     <t>961-712331-000</t>
   </si>
@@ -478,6 +478,12 @@
   <si>
     <t>mouser, ! update of component (see build description)</t>
   </si>
+  <si>
+    <t>The 40-pin header cable is missing in the BOM, and also the negative bit that goes on the PCB.</t>
+  </si>
+  <si>
+    <t>This item is referenced as 40-pin IDC cable in the instructions, but does not show as such on adafruit</t>
+  </si>
 </sst>
 </file>
 
@@ -488,12 +494,26 @@
     <numFmt numFmtId="165" formatCode="###0.00;###0.00"/>
     <numFmt numFmtId="166" formatCode="###0.000;###0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -572,130 +592,142 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1572,8 +1604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.3984375" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -1620,10 +1652,10 @@
       <c r="B3" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="35"/>
+      <c r="D3" s="36"/>
       <c r="E3" s="6">
         <v>35</v>
       </c>
@@ -1647,10 +1679,10 @@
       <c r="B4" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="10">
         <v>9.89</v>
       </c>
@@ -1674,10 +1706,10 @@
       <c r="B5" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="37"/>
       <c r="E5" s="10">
         <v>60</v>
       </c>
@@ -1701,8 +1733,8 @@
       <c r="B6" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="10">
         <v>1.54</v>
       </c>
@@ -1729,10 +1761,10 @@
       <c r="B7" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="36"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="10">
         <v>18.5</v>
       </c>
@@ -1756,10 +1788,10 @@
       <c r="B8" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="36"/>
+      <c r="D8" s="37"/>
       <c r="E8" s="10">
         <v>42</v>
       </c>
@@ -1783,10 +1815,10 @@
       <c r="B9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="36"/>
+      <c r="D9" s="37"/>
       <c r="E9" s="10">
         <v>36.299999999999997</v>
       </c>
@@ -1810,10 +1842,10 @@
       <c r="B10" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="37"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="10">
         <v>65</v>
       </c>
@@ -1837,10 +1869,10 @@
       <c r="B11" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="38">
         <v>237825</v>
       </c>
-      <c r="D11" s="37"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="10">
         <v>9.9499999999999993</v>
       </c>
@@ -1864,10 +1896,10 @@
       <c r="B12" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="36"/>
+      <c r="D12" s="37"/>
       <c r="E12" s="9" t="s">
         <v>83</v>
       </c>
@@ -1891,10 +1923,10 @@
       <c r="B13" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="36"/>
+      <c r="D13" s="37"/>
       <c r="E13" s="10">
         <v>25</v>
       </c>
@@ -1918,10 +1950,10 @@
       <c r="B14" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="36"/>
+      <c r="D14" s="37"/>
       <c r="E14" s="9">
         <v>32.869999999999997</v>
       </c>
@@ -1945,10 +1977,10 @@
       <c r="B15" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="36"/>
+      <c r="D15" s="37"/>
       <c r="E15" s="10">
         <v>10.68</v>
       </c>
@@ -1972,10 +2004,10 @@
       <c r="B16" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="36"/>
+      <c r="D16" s="37"/>
       <c r="E16" s="9">
         <v>5.62</v>
       </c>
@@ -1999,10 +2031,10 @@
       <c r="B17" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="38"/>
+      <c r="D17" s="39"/>
       <c r="E17" s="16">
         <v>0.56999999999999995</v>
       </c>
@@ -2026,10 +2058,10 @@
       <c r="B18" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="36"/>
+      <c r="D18" s="37"/>
       <c r="E18" s="9" t="s">
         <v>93</v>
       </c>
@@ -2053,10 +2085,10 @@
       <c r="B19" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="36"/>
+      <c r="D19" s="37"/>
       <c r="E19" s="10">
         <v>0.11</v>
       </c>
@@ -2080,10 +2112,10 @@
       <c r="B20" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="38"/>
+      <c r="D20" s="39"/>
       <c r="E20" s="17">
         <v>0.25</v>
       </c>
@@ -2107,10 +2139,10 @@
       <c r="B21" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="38"/>
+      <c r="D21" s="39"/>
       <c r="E21" s="17">
         <v>0.1</v>
       </c>
@@ -2131,13 +2163,13 @@
       <c r="A22" s="12">
         <v>20</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C22" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="36"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="10">
         <v>1.25</v>
       </c>
@@ -2158,13 +2190,13 @@
       <c r="A23" s="12">
         <v>21</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="37">
+      <c r="C23" s="38">
         <v>856</v>
       </c>
-      <c r="D23" s="37"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="9">
         <v>3.75</v>
       </c>
@@ -2179,6 +2211,9 @@
       </c>
       <c r="I23" s="7" t="s">
         <v>53</v>
+      </c>
+      <c r="J23" s="43" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:13" s="8" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -2188,10 +2223,10 @@
       <c r="B24" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="36"/>
+      <c r="D24" s="37"/>
       <c r="E24" s="10">
         <v>0.15</v>
       </c>
@@ -2215,10 +2250,10 @@
       <c r="B25" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="37">
+      <c r="C25" s="38">
         <v>2222</v>
       </c>
-      <c r="D25" s="37"/>
+      <c r="D25" s="38"/>
       <c r="E25" s="10">
         <v>1</v>
       </c>
@@ -2233,6 +2268,9 @@
       </c>
       <c r="I25" s="7" t="s">
         <v>53</v>
+      </c>
+      <c r="J25" s="43" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="8" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
@@ -2242,10 +2280,10 @@
       <c r="B26" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="36" t="s">
+      <c r="C26" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="36"/>
+      <c r="D26" s="37"/>
       <c r="E26" s="10">
         <v>0.09</v>
       </c>
@@ -2269,10 +2307,10 @@
       <c r="B27" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="36"/>
+      <c r="D27" s="37"/>
       <c r="E27" s="10">
         <v>0.28999999999999998</v>
       </c>
@@ -2302,10 +2340,10 @@
       <c r="B28" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="36"/>
+      <c r="D28" s="37"/>
       <c r="E28" s="10">
         <v>0.79</v>
       </c>
@@ -2335,10 +2373,10 @@
       <c r="B29" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C29" s="36">
+      <c r="C29" s="37">
         <v>1952370</v>
       </c>
-      <c r="D29" s="36"/>
+      <c r="D29" s="37"/>
       <c r="E29" s="9">
         <v>18.95</v>
       </c>
@@ -2362,10 +2400,10 @@
       <c r="B30" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C30" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="D30" s="39"/>
+      <c r="D30" s="41"/>
       <c r="E30" s="22">
         <v>0.43</v>
       </c>
@@ -2389,10 +2427,10 @@
       <c r="B31" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="36"/>
+      <c r="D31" s="37"/>
       <c r="E31" s="10">
         <v>1.28</v>
       </c>
@@ -2433,10 +2471,10 @@
       <c r="B33" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="36" t="s">
+      <c r="C33" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="36"/>
+      <c r="D33" s="37"/>
       <c r="E33" s="9">
         <v>1.25</v>
       </c>
@@ -2460,10 +2498,10 @@
       <c r="B34" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C34" s="37">
+      <c r="C34" s="38">
         <v>2094346</v>
       </c>
-      <c r="D34" s="37"/>
+      <c r="D34" s="38"/>
       <c r="E34" s="26">
         <v>6.9000000000000006E-2</v>
       </c>
@@ -2487,10 +2525,10 @@
       <c r="B35" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="37">
+      <c r="C35" s="38">
         <v>106797</v>
       </c>
-      <c r="D35" s="37"/>
+      <c r="D35" s="38"/>
       <c r="E35" s="26">
         <v>7.9000000000000001E-2</v>
       </c>
@@ -2514,10 +2552,10 @@
       <c r="B36" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="37">
+      <c r="C36" s="38">
         <v>106810</v>
       </c>
-      <c r="D36" s="37"/>
+      <c r="D36" s="38"/>
       <c r="E36" s="26">
         <v>7.9000000000000001E-2</v>
       </c>
@@ -2541,10 +2579,10 @@
       <c r="B37" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="37">
+      <c r="C37" s="38">
         <v>38173</v>
       </c>
-      <c r="D37" s="37"/>
+      <c r="D37" s="38"/>
       <c r="E37" s="26">
         <v>9.9000000000000005E-2</v>
       </c>
@@ -2568,10 +2606,10 @@
       <c r="B38" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C38" s="36">
+      <c r="C38" s="37">
         <v>51553</v>
       </c>
-      <c r="D38" s="36"/>
+      <c r="D38" s="37"/>
       <c r="E38" s="26">
         <v>5.8999999999999997E-2</v>
       </c>
@@ -2595,10 +2633,10 @@
       <c r="B39" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C39" s="37">
+      <c r="C39" s="38">
         <v>40943</v>
       </c>
-      <c r="D39" s="37"/>
+      <c r="D39" s="38"/>
       <c r="E39" s="9">
         <v>5.8999999999999997E-2</v>
       </c>
@@ -2622,10 +2660,10 @@
       <c r="B40" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C40" s="36">
+      <c r="C40" s="37">
         <v>38165</v>
       </c>
-      <c r="D40" s="36"/>
+      <c r="D40" s="37"/>
       <c r="E40" s="9">
         <v>5.8999999999999997E-2</v>
       </c>
@@ -2649,10 +2687,10 @@
       <c r="B41" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C41" s="37">
+      <c r="C41" s="38">
         <v>106850</v>
       </c>
-      <c r="D41" s="37"/>
+      <c r="D41" s="38"/>
       <c r="E41" s="26">
         <v>5.8999999999999997E-2</v>
       </c>
@@ -2676,10 +2714,10 @@
       <c r="B42" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C42" s="37">
+      <c r="C42" s="38">
         <v>106826</v>
       </c>
-      <c r="D42" s="37"/>
+      <c r="D42" s="38"/>
       <c r="E42" s="9">
         <v>6.5000000000000002E-2</v>
       </c>
@@ -2703,10 +2741,10 @@
       <c r="B43" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C43" s="36" t="s">
+      <c r="C43" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="D43" s="36"/>
+      <c r="D43" s="37"/>
       <c r="E43" s="10">
         <v>0.56000000000000005</v>
       </c>
@@ -2733,10 +2771,10 @@
       <c r="B44" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C44" s="36" t="s">
+      <c r="C44" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D44" s="36"/>
+      <c r="D44" s="37"/>
       <c r="E44" s="10">
         <v>0.61</v>
       </c>
@@ -2763,10 +2801,10 @@
       <c r="B45" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C45" s="36" t="s">
+      <c r="C45" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="D45" s="36"/>
+      <c r="D45" s="37"/>
       <c r="E45" s="10">
         <v>0.54</v>
       </c>
@@ -2793,10 +2831,10 @@
       <c r="B46" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C46" s="36" t="s">
+      <c r="C46" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D46" s="36"/>
+      <c r="D46" s="37"/>
       <c r="E46" s="10">
         <v>0.27</v>
       </c>
@@ -2823,10 +2861,10 @@
       <c r="B47" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="C47" s="40" t="s">
+      <c r="C47" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="D47" s="40"/>
+      <c r="D47" s="42"/>
       <c r="E47" s="27">
         <v>0.41799999999999998</v>
       </c>
@@ -2853,10 +2891,10 @@
       <c r="B48" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="C48" s="40" t="s">
+      <c r="C48" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D48" s="40"/>
+      <c r="D48" s="42"/>
       <c r="E48" s="27">
         <v>0.246</v>
       </c>
@@ -2880,10 +2918,10 @@
       <c r="B49" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="C49" s="40" t="s">
+      <c r="C49" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D49" s="40"/>
+      <c r="D49" s="42"/>
       <c r="E49" s="27">
         <v>0.246</v>
       </c>
@@ -2907,10 +2945,10 @@
       <c r="B50" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C50" s="36">
+      <c r="C50" s="37">
         <v>2135064</v>
       </c>
-      <c r="D50" s="36"/>
+      <c r="D50" s="37"/>
       <c r="E50" s="10">
         <v>2.4900000000000002</v>
       </c>
@@ -2934,10 +2972,10 @@
       <c r="B51" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="40" t="s">
+      <c r="C51" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="D51" s="40"/>
+      <c r="D51" s="42"/>
       <c r="E51" s="12">
         <v>67</v>
       </c>
@@ -2961,8 +2999,8 @@
       <c r="B52" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
       <c r="E52" s="10">
         <v>9.99</v>
       </c>
@@ -2989,10 +3027,10 @@
       <c r="B53" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C53" s="40" t="s">
+      <c r="C53" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="D53" s="40"/>
+      <c r="D53" s="42"/>
       <c r="E53" s="13"/>
       <c r="F53" s="15">
         <v>5</v>
@@ -3012,10 +3050,10 @@
       <c r="B54" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="C54" s="39" t="s">
+      <c r="C54" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="D54" s="39"/>
+      <c r="D54" s="41"/>
       <c r="E54" s="21"/>
       <c r="F54" s="29">
         <v>5</v>
@@ -3033,10 +3071,10 @@
       <c r="B55" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="C55" s="39" t="s">
+      <c r="C55" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="D55" s="39"/>
+      <c r="D55" s="41"/>
       <c r="E55" s="21"/>
       <c r="F55" s="21"/>
       <c r="G55" s="21"/>
@@ -3054,10 +3092,10 @@
       <c r="B56" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="C56" s="39" t="s">
+      <c r="C56" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="D56" s="39"/>
+      <c r="D56" s="41"/>
       <c r="E56" s="21"/>
       <c r="F56" s="21"/>
       <c r="G56" s="21"/>

</xml_diff>